<commit_message>
added more EEPROM settings
</commit_message>
<xml_diff>
--- a/Geogram ONE EEPROM Map.xlsx
+++ b/Geogram ONE EEPROM Map.xlsx
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D53" authorId="0">
+    <comment ref="D48" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D55" authorId="0">
+    <comment ref="D50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>ACTIVE 1</t>
   </si>
@@ -249,18 +249,6 @@
     <t>BATT LOW</t>
   </si>
   <si>
-    <t>ACC INT 1</t>
-  </si>
-  <si>
-    <t>ACC INT 2</t>
-  </si>
-  <si>
-    <t>SENS 1</t>
-  </si>
-  <si>
-    <t>SENS 2</t>
-  </si>
-  <si>
     <t>INT ON/OFF</t>
   </si>
   <si>
@@ -315,9 +303,6 @@
     <t>Metric/Standard</t>
   </si>
   <si>
-    <t>ACC other</t>
-  </si>
-  <si>
     <t>Geo data format</t>
   </si>
   <si>
@@ -373,6 +358,51 @@
   </si>
   <si>
     <t>RESET3</t>
+  </si>
+  <si>
+    <t>BMA - 0x10</t>
+  </si>
+  <si>
+    <t>BMA - 0x11</t>
+  </si>
+  <si>
+    <t>BMA - 0x0F</t>
+  </si>
+  <si>
+    <t>BMA - 0x16</t>
+  </si>
+  <si>
+    <t>BMA - 0x17</t>
+  </si>
+  <si>
+    <t>BMA - 0x19</t>
+  </si>
+  <si>
+    <t>BMA - 0x1B</t>
+  </si>
+  <si>
+    <t>BMA - 0x20</t>
+  </si>
+  <si>
+    <t>BMA - 0x21</t>
+  </si>
+  <si>
+    <t>BMA - 0x25</t>
+  </si>
+  <si>
+    <t>BMA - 0x26</t>
+  </si>
+  <si>
+    <t>BMA - 0x27</t>
+  </si>
+  <si>
+    <t>BMA - 0x28</t>
+  </si>
+  <si>
+    <t>BMA - 0x1A</t>
+  </si>
+  <si>
+    <t>Speed Message</t>
   </si>
 </sst>
 </file>
@@ -534,8 +564,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -543,21 +576,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -569,12 +605,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,27 +902,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="V1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>34</v>
+      <c r="B2" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -903,14 +933,14 @@
       <c r="E2">
         <v>200</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>63</v>
+      <c r="F2" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="G2">
         <v>300</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>67</v>
+      <c r="H2" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="I2">
         <v>400</v>
@@ -931,7 +961,7 @@
         <v>900</v>
       </c>
       <c r="V2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -942,24 +972,24 @@
         <f>A2+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="10"/>
       <c r="C3">
         <f>C2+1</f>
         <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <f>E2+1</f>
         <v>201</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="5"/>
       <c r="G3">
         <f>G2+1</f>
         <v>301</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="5"/>
       <c r="I3">
         <f>I2+1</f>
         <v>401</v>
@@ -985,7 +1015,7 @@
         <v>901</v>
       </c>
       <c r="V3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="X3">
         <v>1</v>
@@ -996,7 +1026,7 @@
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="10"/>
       <c r="C4">
         <f t="shared" ref="C4:C67" si="1">C3+1</f>
         <v>102</v>
@@ -1008,12 +1038,12 @@
         <f t="shared" ref="E4:E67" si="2">E3+1</f>
         <v>202</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="5"/>
       <c r="G4">
         <f t="shared" ref="G4:G67" si="3">G3+1</f>
         <v>302</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="5"/>
       <c r="I4">
         <f t="shared" ref="I4:I67" si="4">I3+1</f>
         <v>402</v>
@@ -1050,24 +1080,24 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="10"/>
       <c r="C5">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
         <v>203</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="5"/>
       <c r="G5">
         <f t="shared" si="3"/>
         <v>303</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="5"/>
       <c r="I5">
         <f t="shared" si="4"/>
         <v>403</v>
@@ -1104,22 +1134,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="10"/>
       <c r="C6">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="9"/>
       <c r="E6">
         <f t="shared" si="2"/>
         <v>204</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="5"/>
       <c r="G6">
         <f t="shared" si="3"/>
         <v>304</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="5"/>
       <c r="I6">
         <f t="shared" si="4"/>
         <v>404</v>
@@ -1156,24 +1186,24 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>35</v>
+      <c r="B7" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="9"/>
       <c r="E7">
         <f t="shared" si="2"/>
         <v>205</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="5"/>
       <c r="G7">
         <f t="shared" si="3"/>
         <v>305</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="5"/>
       <c r="I7">
         <f t="shared" si="4"/>
         <v>405</v>
@@ -1199,7 +1229,7 @@
         <v>905</v>
       </c>
       <c r="V7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="X7">
         <v>5</v>
@@ -1210,22 +1240,22 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="13"/>
       <c r="C8">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="8"/>
       <c r="E8">
         <f t="shared" si="2"/>
         <v>206</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="5"/>
       <c r="G8">
         <f t="shared" si="3"/>
         <v>306</v>
       </c>
-      <c r="H8" s="19"/>
+      <c r="H8" s="5"/>
       <c r="I8">
         <f t="shared" si="4"/>
         <v>406</v>
@@ -1251,7 +1281,7 @@
         <v>906</v>
       </c>
       <c r="V8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="X8">
         <v>6</v>
@@ -1262,24 +1292,24 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="13"/>
       <c r="C9">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
         <v>207</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="5"/>
       <c r="G9">
         <f t="shared" si="3"/>
         <v>307</v>
       </c>
-      <c r="H9" s="19"/>
+      <c r="H9" s="5"/>
       <c r="I9">
         <f t="shared" si="4"/>
         <v>407</v>
@@ -1305,7 +1335,7 @@
         <v>907</v>
       </c>
       <c r="V9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="X9">
         <v>7</v>
@@ -1316,22 +1346,22 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="13"/>
       <c r="C10">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="12"/>
       <c r="E10">
         <f t="shared" si="2"/>
         <v>208</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="5"/>
       <c r="G10">
         <f t="shared" si="3"/>
         <v>308</v>
       </c>
-      <c r="H10" s="19"/>
+      <c r="H10" s="5"/>
       <c r="I10">
         <f t="shared" si="4"/>
         <v>408</v>
@@ -1362,22 +1392,22 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="13"/>
       <c r="C11">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="12"/>
       <c r="E11">
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="5"/>
       <c r="G11">
         <f t="shared" si="3"/>
         <v>309</v>
       </c>
-      <c r="H11" s="19"/>
+      <c r="H11" s="5"/>
       <c r="I11">
         <f t="shared" si="4"/>
         <v>409</v>
@@ -1408,22 +1438,22 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="13"/>
       <c r="C12">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="12"/>
       <c r="E12">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="F12" s="19"/>
+      <c r="F12" s="5"/>
       <c r="G12">
         <f t="shared" si="3"/>
         <v>310</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="5"/>
       <c r="I12">
         <f t="shared" si="4"/>
         <v>410</v>
@@ -1449,7 +1479,7 @@
         <v>910</v>
       </c>
       <c r="V12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -1457,24 +1487,24 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="13"/>
       <c r="C13">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
         <v>211</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="5"/>
       <c r="G13">
         <f t="shared" si="3"/>
         <v>311</v>
       </c>
-      <c r="H13" s="19"/>
+      <c r="H13" s="5"/>
       <c r="I13">
         <f t="shared" si="4"/>
         <v>411</v>
@@ -1500,7 +1530,7 @@
         <v>911</v>
       </c>
       <c r="V13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1508,22 +1538,22 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="13"/>
       <c r="C14">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="12"/>
       <c r="E14">
         <f t="shared" si="2"/>
         <v>212</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="5"/>
       <c r="G14">
         <f t="shared" si="3"/>
         <v>312</v>
       </c>
-      <c r="H14" s="19"/>
+      <c r="H14" s="5"/>
       <c r="I14">
         <f t="shared" si="4"/>
         <v>412</v>
@@ -1549,7 +1579,7 @@
         <v>912</v>
       </c>
       <c r="V14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1557,22 +1587,22 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="13"/>
       <c r="C15">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="12"/>
       <c r="E15">
         <f t="shared" si="2"/>
         <v>213</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="5"/>
       <c r="G15">
         <f t="shared" si="3"/>
         <v>313</v>
       </c>
-      <c r="H15" s="19"/>
+      <c r="H15" s="5"/>
       <c r="I15">
         <f t="shared" si="4"/>
         <v>413</v>
@@ -1598,7 +1628,7 @@
         <v>913</v>
       </c>
       <c r="V15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -1606,22 +1636,22 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="13"/>
       <c r="C16">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="12"/>
       <c r="E16">
         <f t="shared" si="2"/>
         <v>214</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="5"/>
       <c r="G16">
         <f t="shared" si="3"/>
         <v>314</v>
       </c>
-      <c r="H16" s="19"/>
+      <c r="H16" s="5"/>
       <c r="I16">
         <f t="shared" si="4"/>
         <v>414</v>
@@ -1647,7 +1677,7 @@
         <v>914</v>
       </c>
       <c r="V16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1655,7 +1685,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="13"/>
       <c r="C17">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1667,12 +1697,12 @@
         <f t="shared" si="2"/>
         <v>215</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="5"/>
       <c r="G17">
         <f t="shared" si="3"/>
         <v>315</v>
       </c>
-      <c r="H17" s="19"/>
+      <c r="H17" s="5"/>
       <c r="I17">
         <f t="shared" si="4"/>
         <v>415</v>
@@ -1703,24 +1733,24 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="13"/>
       <c r="C18">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
         <v>216</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="5"/>
       <c r="G18">
         <f t="shared" si="3"/>
         <v>316</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="5"/>
       <c r="I18">
         <f t="shared" si="4"/>
         <v>416</v>
@@ -1751,7 +1781,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="13"/>
       <c r="C19">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1763,12 +1793,12 @@
         <f t="shared" si="2"/>
         <v>217</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="5"/>
       <c r="G19">
         <f t="shared" si="3"/>
         <v>317</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="5"/>
       <c r="I19">
         <f t="shared" si="4"/>
         <v>417</v>
@@ -1799,24 +1829,24 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="13"/>
       <c r="C20">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="16" t="s">
         <v>7</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
         <v>218</v>
       </c>
-      <c r="F20" s="19"/>
+      <c r="F20" s="5"/>
       <c r="G20">
         <f t="shared" si="3"/>
         <v>318</v>
       </c>
-      <c r="H20" s="19"/>
+      <c r="H20" s="5"/>
       <c r="I20">
         <f t="shared" si="4"/>
         <v>418</v>
@@ -1847,22 +1877,22 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="13"/>
       <c r="C21">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="17"/>
       <c r="E21">
         <f t="shared" si="2"/>
         <v>219</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="5"/>
       <c r="G21">
         <f t="shared" si="3"/>
         <v>319</v>
       </c>
-      <c r="H21" s="19"/>
+      <c r="H21" s="5"/>
       <c r="I21">
         <f t="shared" si="4"/>
         <v>419</v>
@@ -1893,22 +1923,22 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="13"/>
       <c r="C22">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="18"/>
       <c r="E22">
         <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="5"/>
       <c r="G22">
         <f t="shared" si="3"/>
         <v>320</v>
       </c>
-      <c r="H22" s="19"/>
+      <c r="H22" s="5"/>
       <c r="I22">
         <f t="shared" si="4"/>
         <v>420</v>
@@ -1939,22 +1969,22 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="13"/>
       <c r="C23">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="19"/>
       <c r="E23">
         <f t="shared" si="2"/>
         <v>221</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="5"/>
       <c r="G23">
         <f t="shared" si="3"/>
         <v>321</v>
       </c>
-      <c r="H23" s="19"/>
+      <c r="H23" s="5"/>
       <c r="I23">
         <f t="shared" si="4"/>
         <v>421</v>
@@ -1985,24 +2015,24 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="13"/>
       <c r="C24">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
         <v>222</v>
       </c>
-      <c r="F24" s="19"/>
+      <c r="F24" s="5"/>
       <c r="G24">
         <f t="shared" si="3"/>
         <v>322</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="5"/>
       <c r="I24">
         <f t="shared" si="4"/>
         <v>422</v>
@@ -2033,22 +2063,22 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="13"/>
       <c r="C25">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="15"/>
       <c r="E25">
         <f t="shared" si="2"/>
         <v>223</v>
       </c>
-      <c r="F25" s="19"/>
+      <c r="F25" s="5"/>
       <c r="G25">
         <f t="shared" si="3"/>
         <v>323</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="5"/>
       <c r="I25">
         <f t="shared" si="4"/>
         <v>423</v>
@@ -2079,22 +2109,22 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="13"/>
       <c r="C26">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="15"/>
       <c r="E26">
         <f t="shared" si="2"/>
         <v>224</v>
       </c>
-      <c r="F26" s="19"/>
+      <c r="F26" s="5"/>
       <c r="G26">
         <f t="shared" si="3"/>
         <v>324</v>
       </c>
-      <c r="H26" s="19"/>
+      <c r="H26" s="5"/>
       <c r="I26">
         <f t="shared" si="4"/>
         <v>424</v>
@@ -2125,22 +2155,25 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="13"/>
       <c r="C27">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="15"/>
       <c r="E27">
         <f t="shared" si="2"/>
         <v>225</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>64</v>
+      <c r="F27" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
         <v>325</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="I27">
         <f t="shared" si="4"/>
@@ -2172,23 +2205,24 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="14"/>
       <c r="C28">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
         <v>226</v>
       </c>
-      <c r="F28" s="19"/>
+      <c r="F28" s="5"/>
       <c r="G28">
         <f t="shared" si="3"/>
         <v>326</v>
       </c>
+      <c r="H28" s="5"/>
       <c r="I28">
         <f t="shared" si="4"/>
         <v>426</v>
@@ -2219,21 +2253,22 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="14"/>
       <c r="C29">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="15"/>
       <c r="E29">
         <f t="shared" si="2"/>
         <v>227</v>
       </c>
-      <c r="F29" s="19"/>
+      <c r="F29" s="5"/>
       <c r="G29">
         <f t="shared" si="3"/>
         <v>327</v>
       </c>
+      <c r="H29" s="5"/>
       <c r="I29">
         <f t="shared" si="4"/>
         <v>427</v>
@@ -2264,21 +2299,22 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="14"/>
       <c r="C30">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="15"/>
       <c r="E30">
         <f t="shared" si="2"/>
         <v>228</v>
       </c>
-      <c r="F30" s="19"/>
+      <c r="F30" s="5"/>
       <c r="G30">
         <f t="shared" si="3"/>
         <v>328</v>
       </c>
+      <c r="H30" s="5"/>
       <c r="I30">
         <f t="shared" si="4"/>
         <v>428</v>
@@ -2309,21 +2345,22 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="14"/>
       <c r="C31">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="15"/>
       <c r="E31">
         <f t="shared" si="2"/>
         <v>229</v>
       </c>
-      <c r="F31" s="19"/>
+      <c r="F31" s="5"/>
       <c r="G31">
         <f t="shared" si="3"/>
         <v>329</v>
       </c>
+      <c r="H31" s="5"/>
       <c r="I31">
         <f t="shared" si="4"/>
         <v>429</v>
@@ -2354,7 +2391,7 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="14"/>
       <c r="C32">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -2366,11 +2403,12 @@
         <f t="shared" si="2"/>
         <v>230</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="5"/>
       <c r="G32">
         <f t="shared" si="3"/>
         <v>330</v>
       </c>
+      <c r="H32" s="5"/>
       <c r="I32">
         <f t="shared" si="4"/>
         <v>430</v>
@@ -2401,23 +2439,24 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="13"/>
+      <c r="B33" s="14"/>
       <c r="C33">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
         <v>231</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="5"/>
       <c r="G33">
         <f t="shared" si="3"/>
         <v>331</v>
       </c>
+      <c r="H33" s="5"/>
       <c r="I33">
         <f t="shared" si="4"/>
         <v>431</v>
@@ -2448,7 +2487,7 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="13"/>
+      <c r="B34" s="14"/>
       <c r="C34">
         <f t="shared" si="1"/>
         <v>132</v>
@@ -2460,11 +2499,12 @@
         <f t="shared" si="2"/>
         <v>232</v>
       </c>
-      <c r="F34" s="19"/>
+      <c r="F34" s="5"/>
       <c r="G34">
         <f t="shared" si="3"/>
         <v>332</v>
       </c>
+      <c r="H34" s="5"/>
       <c r="I34">
         <f t="shared" si="4"/>
         <v>432</v>
@@ -2495,23 +2535,24 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="13"/>
+      <c r="B35" s="14"/>
       <c r="C35">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E35">
         <f t="shared" si="2"/>
         <v>233</v>
       </c>
-      <c r="F35" s="19"/>
+      <c r="F35" s="5"/>
       <c r="G35">
         <f t="shared" si="3"/>
         <v>333</v>
       </c>
+      <c r="H35" s="5"/>
       <c r="I35">
         <f t="shared" si="4"/>
         <v>433</v>
@@ -2542,21 +2583,22 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="13"/>
+      <c r="B36" s="14"/>
       <c r="C36">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="9"/>
       <c r="E36">
         <f t="shared" si="2"/>
         <v>234</v>
       </c>
-      <c r="F36" s="19"/>
+      <c r="F36" s="5"/>
       <c r="G36">
         <f t="shared" si="3"/>
         <v>334</v>
       </c>
+      <c r="H36" s="5"/>
       <c r="I36">
         <f t="shared" si="4"/>
         <v>434</v>
@@ -2587,21 +2629,22 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="14"/>
       <c r="C37">
         <f t="shared" si="1"/>
         <v>135</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="9"/>
       <c r="E37">
         <f t="shared" si="2"/>
         <v>235</v>
       </c>
-      <c r="F37" s="19"/>
+      <c r="F37" s="5"/>
       <c r="G37">
         <f t="shared" si="3"/>
         <v>335</v>
       </c>
+      <c r="H37" s="5"/>
       <c r="I37">
         <f t="shared" si="4"/>
         <v>435</v>
@@ -2632,21 +2675,22 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="14"/>
       <c r="C38">
         <f t="shared" si="1"/>
         <v>136</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="8"/>
       <c r="E38">
         <f t="shared" si="2"/>
         <v>236</v>
       </c>
-      <c r="F38" s="19"/>
+      <c r="F38" s="5"/>
       <c r="G38">
         <f t="shared" si="3"/>
         <v>336</v>
       </c>
+      <c r="H38" s="5"/>
       <c r="I38">
         <f t="shared" si="4"/>
         <v>436</v>
@@ -2677,23 +2721,24 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="14"/>
       <c r="C39">
         <f t="shared" si="1"/>
         <v>137</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
         <v>237</v>
       </c>
-      <c r="F39" s="19"/>
+      <c r="F39" s="5"/>
       <c r="G39">
         <f t="shared" si="3"/>
         <v>337</v>
       </c>
+      <c r="H39" s="5"/>
       <c r="I39">
         <f t="shared" si="4"/>
         <v>437</v>
@@ -2724,21 +2769,22 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="14"/>
       <c r="C40">
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="18"/>
       <c r="E40">
         <f t="shared" si="2"/>
         <v>238</v>
       </c>
-      <c r="F40" s="19"/>
+      <c r="F40" s="5"/>
       <c r="G40">
         <f t="shared" si="3"/>
         <v>338</v>
       </c>
+      <c r="H40" s="5"/>
       <c r="I40">
         <f t="shared" si="4"/>
         <v>438</v>
@@ -2769,21 +2815,22 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="13"/>
+      <c r="B41" s="14"/>
       <c r="C41">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="18"/>
       <c r="E41">
         <f t="shared" si="2"/>
         <v>239</v>
       </c>
-      <c r="F41" s="19"/>
+      <c r="F41" s="5"/>
       <c r="G41">
         <f t="shared" si="3"/>
         <v>339</v>
       </c>
+      <c r="H41" s="5"/>
       <c r="I41">
         <f t="shared" si="4"/>
         <v>439</v>
@@ -2814,21 +2861,22 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" s="13"/>
+      <c r="B42" s="14"/>
       <c r="C42">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="D42" s="17"/>
+      <c r="D42" s="19"/>
       <c r="E42">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="F42" s="19"/>
+      <c r="F42" s="5"/>
       <c r="G42">
         <f t="shared" si="3"/>
         <v>340</v>
       </c>
+      <c r="H42" s="5"/>
       <c r="I42">
         <f t="shared" si="4"/>
         <v>440</v>
@@ -2859,23 +2907,24 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="13"/>
+      <c r="B43" s="14"/>
       <c r="C43">
         <f t="shared" si="1"/>
         <v>141</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E43">
         <f t="shared" si="2"/>
         <v>241</v>
       </c>
-      <c r="F43" s="19"/>
+      <c r="F43" s="5"/>
       <c r="G43">
         <f t="shared" si="3"/>
         <v>341</v>
       </c>
+      <c r="H43" s="5"/>
       <c r="I43">
         <f t="shared" si="4"/>
         <v>441</v>
@@ -2906,21 +2955,22 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="13"/>
+      <c r="B44" s="14"/>
       <c r="C44">
         <f t="shared" si="1"/>
         <v>142</v>
       </c>
-      <c r="D44" s="6"/>
+      <c r="D44" s="7"/>
       <c r="E44">
         <f t="shared" si="2"/>
         <v>242</v>
       </c>
-      <c r="F44" s="19"/>
+      <c r="F44" s="5"/>
       <c r="G44">
         <f t="shared" si="3"/>
         <v>342</v>
       </c>
+      <c r="H44" s="5"/>
       <c r="I44">
         <f t="shared" si="4"/>
         <v>442</v>
@@ -2951,21 +3001,22 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B45" s="13"/>
+      <c r="B45" s="14"/>
       <c r="C45">
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
-      <c r="D45" s="6"/>
+      <c r="D45" s="7"/>
       <c r="E45">
         <f t="shared" si="2"/>
         <v>243</v>
       </c>
-      <c r="F45" s="19"/>
+      <c r="F45" s="5"/>
       <c r="G45">
         <f t="shared" si="3"/>
         <v>343</v>
       </c>
+      <c r="H45" s="5"/>
       <c r="I45">
         <f t="shared" si="4"/>
         <v>443</v>
@@ -2996,23 +3047,24 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B46" s="9" t="s">
-        <v>36</v>
+      <c r="B46" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
         <v>144</v>
       </c>
-      <c r="D46" s="11"/>
+      <c r="D46" s="8"/>
       <c r="E46">
         <f t="shared" si="2"/>
         <v>244</v>
       </c>
-      <c r="F46" s="19"/>
+      <c r="F46" s="5"/>
       <c r="G46">
         <f t="shared" si="3"/>
         <v>344</v>
       </c>
+      <c r="H46" s="5"/>
       <c r="I46">
         <f t="shared" si="4"/>
         <v>444</v>
@@ -3043,23 +3095,24 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B47" s="9"/>
+      <c r="B47" s="11"/>
       <c r="C47">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E47">
         <f t="shared" si="2"/>
         <v>245</v>
       </c>
-      <c r="F47" s="19"/>
+      <c r="F47" s="5"/>
       <c r="G47">
         <f t="shared" si="3"/>
         <v>345</v>
       </c>
+      <c r="H47" s="5"/>
       <c r="I47">
         <f t="shared" si="4"/>
         <v>445</v>
@@ -3090,23 +3143,24 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B48" s="11"/>
       <c r="C48">
         <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
         <v>246</v>
       </c>
-      <c r="F48" s="19"/>
+      <c r="F48" s="5"/>
       <c r="G48">
         <f t="shared" si="3"/>
         <v>346</v>
       </c>
+      <c r="H48" s="5"/>
       <c r="I48">
         <f t="shared" si="4"/>
         <v>446</v>
@@ -3137,23 +3191,24 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="11"/>
       <c r="C49">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E49">
         <f t="shared" si="2"/>
         <v>247</v>
       </c>
-      <c r="F49" s="19"/>
+      <c r="F49" s="5"/>
       <c r="G49">
         <f t="shared" si="3"/>
         <v>347</v>
       </c>
+      <c r="H49" s="5"/>
       <c r="I49">
         <f t="shared" si="4"/>
         <v>447</v>
@@ -3184,23 +3239,24 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="11"/>
       <c r="C50">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E50">
         <f t="shared" si="2"/>
         <v>248</v>
       </c>
-      <c r="F50" s="19"/>
+      <c r="F50" s="5"/>
       <c r="G50">
         <f t="shared" si="3"/>
         <v>348</v>
       </c>
+      <c r="H50" s="5"/>
       <c r="I50">
         <f t="shared" si="4"/>
         <v>448</v>
@@ -3231,23 +3287,24 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="9"/>
+      <c r="B51" s="11"/>
       <c r="C51">
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E51">
         <f t="shared" si="2"/>
         <v>249</v>
       </c>
-      <c r="F51" s="19"/>
+      <c r="F51" s="5"/>
       <c r="G51">
         <f t="shared" si="3"/>
         <v>349</v>
       </c>
+      <c r="H51" s="5"/>
       <c r="I51">
         <f t="shared" si="4"/>
         <v>449</v>
@@ -3278,20 +3335,20 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B52" s="9"/>
+      <c r="B52" s="11"/>
       <c r="C52">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="E52">
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="F52" s="18" t="s">
-        <v>65</v>
+      <c r="F52" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G52">
         <f t="shared" si="3"/>
@@ -3327,19 +3384,19 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B53" s="9"/>
+      <c r="B53" s="11"/>
       <c r="C53">
         <f t="shared" si="1"/>
         <v>151</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E53">
         <f t="shared" si="2"/>
         <v>251</v>
       </c>
-      <c r="F53" s="19"/>
+      <c r="F53" s="5"/>
       <c r="G53">
         <f t="shared" si="3"/>
         <v>351</v>
@@ -3374,19 +3431,19 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B54" s="9"/>
+      <c r="B54" s="11"/>
       <c r="C54">
         <f t="shared" si="1"/>
         <v>152</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>48</v>
+      <c r="D54" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E54">
         <f t="shared" si="2"/>
         <v>252</v>
       </c>
-      <c r="F54" s="19"/>
+      <c r="F54" s="5"/>
       <c r="G54">
         <f t="shared" si="3"/>
         <v>352</v>
@@ -3421,19 +3478,19 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B55" s="9"/>
+      <c r="B55" s="11"/>
       <c r="C55">
         <f t="shared" si="1"/>
         <v>153</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>49</v>
+      <c r="D55" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="E55">
         <f t="shared" si="2"/>
         <v>253</v>
       </c>
-      <c r="F55" s="19"/>
+      <c r="F55" s="5"/>
       <c r="G55">
         <f t="shared" si="3"/>
         <v>353</v>
@@ -3468,19 +3525,19 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B56" s="9"/>
+      <c r="B56" s="11"/>
       <c r="C56">
         <f t="shared" si="1"/>
         <v>154</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>50</v>
+      <c r="D56" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="E56">
         <f t="shared" si="2"/>
         <v>254</v>
       </c>
-      <c r="F56" s="19"/>
+      <c r="F56" s="5"/>
       <c r="G56">
         <f t="shared" si="3"/>
         <v>354</v>
@@ -3515,19 +3572,19 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B57" s="9"/>
+      <c r="B57" s="11"/>
       <c r="C57">
         <f t="shared" si="1"/>
         <v>155</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>52</v>
+      <c r="D57" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E57">
         <f t="shared" si="2"/>
         <v>255</v>
       </c>
-      <c r="F57" s="19"/>
+      <c r="F57" s="5"/>
       <c r="G57">
         <f t="shared" si="3"/>
         <v>355</v>
@@ -3562,19 +3619,19 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B58" s="9"/>
+      <c r="B58" s="11"/>
       <c r="C58">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>53</v>
+      <c r="D58" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E58">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="F58" s="19"/>
+      <c r="F58" s="5"/>
       <c r="G58">
         <f t="shared" si="3"/>
         <v>356</v>
@@ -3609,19 +3666,19 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B59" s="9"/>
+      <c r="B59" s="11"/>
       <c r="C59">
         <f t="shared" si="1"/>
         <v>157</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>54</v>
+      <c r="D59" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="E59">
         <f t="shared" si="2"/>
         <v>257</v>
       </c>
-      <c r="F59" s="19"/>
+      <c r="F59" s="5"/>
       <c r="G59">
         <f t="shared" si="3"/>
         <v>357</v>
@@ -3656,19 +3713,19 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B60" s="9"/>
+      <c r="B60" s="11"/>
       <c r="C60">
         <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>55</v>
+      <c r="D60" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="E60">
         <f t="shared" si="2"/>
         <v>258</v>
       </c>
-      <c r="F60" s="19"/>
+      <c r="F60" s="5"/>
       <c r="G60">
         <f t="shared" si="3"/>
         <v>358</v>
@@ -3703,19 +3760,19 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="9"/>
+      <c r="B61" s="11"/>
       <c r="C61">
         <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>56</v>
+      <c r="D61" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="E61">
         <f t="shared" si="2"/>
         <v>259</v>
       </c>
-      <c r="F61" s="19"/>
+      <c r="F61" s="5"/>
       <c r="G61">
         <f t="shared" si="3"/>
         <v>359</v>
@@ -3750,19 +3807,19 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="9"/>
+      <c r="B62" s="11"/>
       <c r="C62">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>59</v>
+      <c r="D62" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E62">
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="F62" s="19"/>
+      <c r="F62" s="5"/>
       <c r="G62">
         <f t="shared" si="3"/>
         <v>360</v>
@@ -3797,19 +3854,19 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="9"/>
+      <c r="B63" s="11"/>
       <c r="C63">
         <f t="shared" si="1"/>
         <v>161</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>62</v>
+      <c r="D63" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E63">
         <f t="shared" si="2"/>
         <v>261</v>
       </c>
-      <c r="F63" s="19"/>
+      <c r="F63" s="5"/>
       <c r="G63">
         <f t="shared" si="3"/>
         <v>361</v>
@@ -3844,16 +3901,19 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="9"/>
+      <c r="B64" s="11"/>
       <c r="C64">
         <f t="shared" si="1"/>
         <v>162</v>
       </c>
+      <c r="D64" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="E64">
         <f t="shared" si="2"/>
         <v>262</v>
       </c>
-      <c r="F64" s="19"/>
+      <c r="F64" s="5"/>
       <c r="G64">
         <f t="shared" si="3"/>
         <v>362</v>
@@ -3888,16 +3948,19 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="9"/>
+      <c r="B65" s="11"/>
       <c r="C65">
         <f t="shared" si="1"/>
         <v>163</v>
       </c>
+      <c r="D65" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E65">
         <f t="shared" si="2"/>
         <v>263</v>
       </c>
-      <c r="F65" s="19"/>
+      <c r="F65" s="5"/>
       <c r="G65">
         <f t="shared" si="3"/>
         <v>363</v>
@@ -3932,16 +3995,17 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="9"/>
+      <c r="B66" s="11"/>
       <c r="C66">
         <f t="shared" si="1"/>
         <v>164</v>
       </c>
+      <c r="D66" s="3"/>
       <c r="E66">
         <f t="shared" si="2"/>
         <v>264</v>
       </c>
-      <c r="F66" s="19"/>
+      <c r="F66" s="5"/>
       <c r="G66">
         <f t="shared" si="3"/>
         <v>364</v>
@@ -3976,16 +4040,17 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="9"/>
+      <c r="B67" s="11"/>
       <c r="C67">
         <f t="shared" si="1"/>
         <v>165</v>
       </c>
+      <c r="D67" s="3"/>
       <c r="E67">
         <f t="shared" si="2"/>
         <v>265</v>
       </c>
-      <c r="F67" s="19"/>
+      <c r="F67" s="5"/>
       <c r="G67">
         <f t="shared" si="3"/>
         <v>365</v>
@@ -4020,16 +4085,19 @@
         <f t="shared" ref="A68:A101" si="10">A67+1</f>
         <v>66</v>
       </c>
-      <c r="B68" s="9"/>
+      <c r="B68" s="11"/>
       <c r="C68">
         <f t="shared" ref="C68:C101" si="11">C67+1</f>
         <v>166</v>
       </c>
+      <c r="D68" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E68">
         <f t="shared" ref="E68:E101" si="12">E67+1</f>
         <v>266</v>
       </c>
-      <c r="F68" s="19"/>
+      <c r="F68" s="5"/>
       <c r="G68">
         <f t="shared" ref="G68:G101" si="13">G67+1</f>
         <v>366</v>
@@ -4064,16 +4132,19 @@
         <f t="shared" si="10"/>
         <v>67</v>
       </c>
-      <c r="B69" s="9"/>
+      <c r="B69" s="11"/>
       <c r="C69">
         <f t="shared" si="11"/>
         <v>167</v>
       </c>
+      <c r="D69" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E69">
         <f t="shared" si="12"/>
         <v>267</v>
       </c>
-      <c r="F69" s="19"/>
+      <c r="F69" s="5"/>
       <c r="G69">
         <f t="shared" si="13"/>
         <v>367</v>
@@ -4108,16 +4179,19 @@
         <f t="shared" si="10"/>
         <v>68</v>
       </c>
-      <c r="B70" s="9"/>
+      <c r="B70" s="11"/>
       <c r="C70">
         <f t="shared" si="11"/>
         <v>168</v>
       </c>
+      <c r="D70" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E70">
         <f t="shared" si="12"/>
         <v>268</v>
       </c>
-      <c r="F70" s="19"/>
+      <c r="F70" s="5"/>
       <c r="G70">
         <f t="shared" si="13"/>
         <v>368</v>
@@ -4152,16 +4226,19 @@
         <f t="shared" si="10"/>
         <v>69</v>
       </c>
-      <c r="B71" s="9"/>
+      <c r="B71" s="11"/>
       <c r="C71">
         <f t="shared" si="11"/>
         <v>169</v>
       </c>
+      <c r="D71" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E71">
         <f t="shared" si="12"/>
         <v>269</v>
       </c>
-      <c r="F71" s="19"/>
+      <c r="F71" s="5"/>
       <c r="G71">
         <f t="shared" si="13"/>
         <v>369</v>
@@ -4196,16 +4273,19 @@
         <f t="shared" si="10"/>
         <v>70</v>
       </c>
-      <c r="B72" s="9"/>
+      <c r="B72" s="11"/>
       <c r="C72">
         <f t="shared" si="11"/>
         <v>170</v>
       </c>
+      <c r="D72" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="E72">
         <f t="shared" si="12"/>
         <v>270</v>
       </c>
-      <c r="F72" s="19"/>
+      <c r="F72" s="5"/>
       <c r="G72">
         <f t="shared" si="13"/>
         <v>370</v>
@@ -4240,16 +4320,19 @@
         <f t="shared" si="10"/>
         <v>71</v>
       </c>
-      <c r="B73" s="9"/>
+      <c r="B73" s="11"/>
       <c r="C73">
         <f t="shared" si="11"/>
         <v>171</v>
       </c>
+      <c r="D73" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E73">
         <f t="shared" si="12"/>
         <v>271</v>
       </c>
-      <c r="F73" s="19"/>
+      <c r="F73" s="5"/>
       <c r="G73">
         <f t="shared" si="13"/>
         <v>371</v>
@@ -4284,16 +4367,19 @@
         <f t="shared" si="10"/>
         <v>72</v>
       </c>
-      <c r="B74" s="9"/>
+      <c r="B74" s="11"/>
       <c r="C74">
         <f t="shared" si="11"/>
         <v>172</v>
       </c>
+      <c r="D74" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="E74">
         <f t="shared" si="12"/>
         <v>272</v>
       </c>
-      <c r="F74" s="19"/>
+      <c r="F74" s="5"/>
       <c r="G74">
         <f t="shared" si="13"/>
         <v>372</v>
@@ -4328,7 +4414,7 @@
         <f t="shared" si="10"/>
         <v>73</v>
       </c>
-      <c r="B75" s="9"/>
+      <c r="B75" s="11"/>
       <c r="C75">
         <f t="shared" si="11"/>
         <v>173</v>
@@ -4337,7 +4423,7 @@
         <f t="shared" si="12"/>
         <v>273</v>
       </c>
-      <c r="F75" s="19"/>
+      <c r="F75" s="5"/>
       <c r="G75">
         <f t="shared" si="13"/>
         <v>373</v>
@@ -4372,7 +4458,7 @@
         <f t="shared" si="10"/>
         <v>74</v>
       </c>
-      <c r="B76" s="9"/>
+      <c r="B76" s="11"/>
       <c r="C76">
         <f t="shared" si="11"/>
         <v>174</v>
@@ -4381,7 +4467,7 @@
         <f t="shared" si="12"/>
         <v>274</v>
       </c>
-      <c r="F76" s="19"/>
+      <c r="F76" s="5"/>
       <c r="G76">
         <f t="shared" si="13"/>
         <v>374</v>
@@ -4416,7 +4502,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="B77" s="9"/>
+      <c r="B77" s="11"/>
       <c r="C77">
         <f t="shared" si="11"/>
         <v>175</v>
@@ -4425,8 +4511,8 @@
         <f t="shared" si="12"/>
         <v>275</v>
       </c>
-      <c r="F77" s="18" t="s">
-        <v>66</v>
+      <c r="F77" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="G77">
         <f t="shared" si="13"/>
@@ -4462,7 +4548,7 @@
         <f t="shared" si="10"/>
         <v>76</v>
       </c>
-      <c r="B78" s="9"/>
+      <c r="B78" s="11"/>
       <c r="C78">
         <f t="shared" si="11"/>
         <v>176</v>
@@ -4471,7 +4557,7 @@
         <f t="shared" si="12"/>
         <v>276</v>
       </c>
-      <c r="F78" s="19"/>
+      <c r="F78" s="5"/>
       <c r="G78">
         <f t="shared" si="13"/>
         <v>376</v>
@@ -4506,7 +4592,7 @@
         <f t="shared" si="10"/>
         <v>77</v>
       </c>
-      <c r="B79" s="9"/>
+      <c r="B79" s="11"/>
       <c r="C79">
         <f t="shared" si="11"/>
         <v>177</v>
@@ -4515,7 +4601,7 @@
         <f t="shared" si="12"/>
         <v>277</v>
       </c>
-      <c r="F79" s="19"/>
+      <c r="F79" s="5"/>
       <c r="G79">
         <f t="shared" si="13"/>
         <v>377</v>
@@ -4550,7 +4636,7 @@
         <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="B80" s="9"/>
+      <c r="B80" s="11"/>
       <c r="C80">
         <f t="shared" si="11"/>
         <v>178</v>
@@ -4559,7 +4645,7 @@
         <f t="shared" si="12"/>
         <v>278</v>
       </c>
-      <c r="F80" s="19"/>
+      <c r="F80" s="5"/>
       <c r="G80">
         <f t="shared" si="13"/>
         <v>378</v>
@@ -4594,7 +4680,7 @@
         <f t="shared" si="10"/>
         <v>79</v>
       </c>
-      <c r="B81" s="9"/>
+      <c r="B81" s="11"/>
       <c r="C81">
         <f t="shared" si="11"/>
         <v>179</v>
@@ -4603,7 +4689,7 @@
         <f t="shared" si="12"/>
         <v>279</v>
       </c>
-      <c r="F81" s="19"/>
+      <c r="F81" s="5"/>
       <c r="G81">
         <f t="shared" si="13"/>
         <v>379</v>
@@ -4638,7 +4724,7 @@
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
-      <c r="B82" s="9"/>
+      <c r="B82" s="11"/>
       <c r="C82">
         <f t="shared" si="11"/>
         <v>180</v>
@@ -4647,7 +4733,7 @@
         <f t="shared" si="12"/>
         <v>280</v>
       </c>
-      <c r="F82" s="19"/>
+      <c r="F82" s="5"/>
       <c r="G82">
         <f t="shared" si="13"/>
         <v>380</v>
@@ -4682,7 +4768,7 @@
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
-      <c r="B83" s="9"/>
+      <c r="B83" s="11"/>
       <c r="C83">
         <f t="shared" si="11"/>
         <v>181</v>
@@ -4691,7 +4777,7 @@
         <f t="shared" si="12"/>
         <v>281</v>
       </c>
-      <c r="F83" s="19"/>
+      <c r="F83" s="5"/>
       <c r="G83">
         <f t="shared" si="13"/>
         <v>381</v>
@@ -4726,7 +4812,7 @@
         <f t="shared" si="10"/>
         <v>82</v>
       </c>
-      <c r="B84" s="9"/>
+      <c r="B84" s="11"/>
       <c r="C84">
         <f t="shared" si="11"/>
         <v>182</v>
@@ -4735,7 +4821,7 @@
         <f t="shared" si="12"/>
         <v>282</v>
       </c>
-      <c r="F84" s="19"/>
+      <c r="F84" s="5"/>
       <c r="G84">
         <f t="shared" si="13"/>
         <v>382</v>
@@ -4770,8 +4856,8 @@
         <f t="shared" si="10"/>
         <v>83</v>
       </c>
-      <c r="B85" s="5" t="s">
-        <v>46</v>
+      <c r="B85" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C85">
         <f t="shared" si="11"/>
@@ -4781,7 +4867,7 @@
         <f t="shared" si="12"/>
         <v>283</v>
       </c>
-      <c r="F85" s="19"/>
+      <c r="F85" s="5"/>
       <c r="G85">
         <f t="shared" si="13"/>
         <v>383</v>
@@ -4816,7 +4902,7 @@
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="B86" s="7"/>
       <c r="C86">
         <f t="shared" si="11"/>
         <v>184</v>
@@ -4825,7 +4911,7 @@
         <f t="shared" si="12"/>
         <v>284</v>
       </c>
-      <c r="F86" s="19"/>
+      <c r="F86" s="5"/>
       <c r="G86">
         <f t="shared" si="13"/>
         <v>384</v>
@@ -4860,7 +4946,7 @@
         <f t="shared" si="10"/>
         <v>85</v>
       </c>
-      <c r="B87" s="6"/>
+      <c r="B87" s="7"/>
       <c r="C87">
         <f t="shared" si="11"/>
         <v>185</v>
@@ -4869,7 +4955,7 @@
         <f t="shared" si="12"/>
         <v>285</v>
       </c>
-      <c r="F87" s="19"/>
+      <c r="F87" s="5"/>
       <c r="G87">
         <f t="shared" si="13"/>
         <v>385</v>
@@ -4904,7 +4990,7 @@
         <f t="shared" si="10"/>
         <v>86</v>
       </c>
-      <c r="B88" s="11"/>
+      <c r="B88" s="8"/>
       <c r="C88">
         <f t="shared" si="11"/>
         <v>186</v>
@@ -4913,7 +4999,7 @@
         <f t="shared" si="12"/>
         <v>286</v>
       </c>
-      <c r="F88" s="19"/>
+      <c r="F88" s="5"/>
       <c r="G88">
         <f t="shared" si="13"/>
         <v>386</v>
@@ -4949,7 +5035,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C89">
         <f t="shared" si="11"/>
@@ -4959,7 +5045,7 @@
         <f t="shared" si="12"/>
         <v>287</v>
       </c>
-      <c r="F89" s="19"/>
+      <c r="F89" s="5"/>
       <c r="G89">
         <f t="shared" si="13"/>
         <v>387</v>
@@ -5005,7 +5091,7 @@
         <f t="shared" si="12"/>
         <v>288</v>
       </c>
-      <c r="F90" s="19"/>
+      <c r="F90" s="5"/>
       <c r="G90">
         <f t="shared" si="13"/>
         <v>388</v>
@@ -5041,7 +5127,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C91">
         <f t="shared" si="11"/>
@@ -5051,7 +5137,7 @@
         <f t="shared" si="12"/>
         <v>289</v>
       </c>
-      <c r="F91" s="19"/>
+      <c r="F91" s="5"/>
       <c r="G91">
         <f t="shared" si="13"/>
         <v>389</v>
@@ -5097,7 +5183,7 @@
         <f t="shared" si="12"/>
         <v>290</v>
       </c>
-      <c r="F92" s="19"/>
+      <c r="F92" s="5"/>
       <c r="G92">
         <f t="shared" si="13"/>
         <v>390</v>
@@ -5143,7 +5229,7 @@
         <f t="shared" si="12"/>
         <v>291</v>
       </c>
-      <c r="F93" s="19"/>
+      <c r="F93" s="5"/>
       <c r="G93">
         <f t="shared" si="13"/>
         <v>391</v>
@@ -5189,7 +5275,7 @@
         <f t="shared" si="12"/>
         <v>292</v>
       </c>
-      <c r="F94" s="19"/>
+      <c r="F94" s="5"/>
       <c r="G94">
         <f t="shared" si="13"/>
         <v>392</v>
@@ -5235,7 +5321,7 @@
         <f t="shared" si="12"/>
         <v>293</v>
       </c>
-      <c r="F95" s="19"/>
+      <c r="F95" s="5"/>
       <c r="G95">
         <f t="shared" si="13"/>
         <v>393</v>
@@ -5281,7 +5367,7 @@
         <f t="shared" si="12"/>
         <v>294</v>
       </c>
-      <c r="F96" s="19"/>
+      <c r="F96" s="5"/>
       <c r="G96">
         <f t="shared" si="13"/>
         <v>394</v>
@@ -5327,7 +5413,7 @@
         <f t="shared" si="12"/>
         <v>295</v>
       </c>
-      <c r="F97" s="19"/>
+      <c r="F97" s="5"/>
       <c r="G97">
         <f t="shared" si="13"/>
         <v>395</v>
@@ -5373,7 +5459,7 @@
         <f t="shared" si="12"/>
         <v>296</v>
       </c>
-      <c r="F98" s="19"/>
+      <c r="F98" s="5"/>
       <c r="G98">
         <f t="shared" si="13"/>
         <v>396</v>
@@ -5419,7 +5505,7 @@
         <f t="shared" si="12"/>
         <v>297</v>
       </c>
-      <c r="F99" s="19"/>
+      <c r="F99" s="5"/>
       <c r="G99">
         <f t="shared" si="13"/>
         <v>397</v>
@@ -5465,7 +5551,7 @@
         <f t="shared" si="12"/>
         <v>298</v>
       </c>
-      <c r="F100" s="19"/>
+      <c r="F100" s="5"/>
       <c r="G100">
         <f t="shared" si="13"/>
         <v>398</v>
@@ -5511,7 +5597,7 @@
         <f t="shared" si="12"/>
         <v>299</v>
       </c>
-      <c r="F101" s="19"/>
+      <c r="F101" s="5"/>
       <c r="G101">
         <f t="shared" si="13"/>
         <v>399</v>
@@ -5542,12 +5628,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="F2:F26"/>
-    <mergeCell ref="F27:F51"/>
-    <mergeCell ref="F52:F76"/>
-    <mergeCell ref="F77:F101"/>
-    <mergeCell ref="H2:H26"/>
+  <mergeCells count="19">
     <mergeCell ref="B85:B88"/>
     <mergeCell ref="D35:D38"/>
     <mergeCell ref="B2:B6"/>
@@ -5561,6 +5642,12 @@
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="D39:D42"/>
+    <mergeCell ref="F2:F26"/>
+    <mergeCell ref="F27:F51"/>
+    <mergeCell ref="F52:F76"/>
+    <mergeCell ref="F77:F101"/>
+    <mergeCell ref="H2:H26"/>
+    <mergeCell ref="H27:H51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
- works.  Getting ready to rewrite PA6C library to use character arrays instead of longs and floats
</commit_message>
<xml_diff>
--- a/Geogram ONE EEPROM Map.xlsx
+++ b/Geogram ONE EEPROM Map.xlsx
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>ACTIVE 1</t>
   </si>
@@ -504,6 +504,30 @@
   </si>
   <si>
     <t>Configure Address</t>
+  </si>
+  <si>
+    <t>IMEI 16 Digits</t>
+  </si>
+  <si>
+    <t>GPRS_APN</t>
+  </si>
+  <si>
+    <t>GPRS USER</t>
+  </si>
+  <si>
+    <t>GPRS PASS</t>
+  </si>
+  <si>
+    <t>PORT</t>
+  </si>
+  <si>
+    <t>GPRS HEADER</t>
+  </si>
+  <si>
+    <t>GPRS REPLY</t>
+  </si>
+  <si>
+    <t>GPRS HOST</t>
   </si>
 </sst>
 </file>
@@ -552,7 +576,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,6 +592,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,31 +666,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -668,16 +691,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -693,7 +706,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="R63" sqref="R63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,7 +1063,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C2">
@@ -1024,35 +1075,39 @@
       <c r="E2">
         <v>200</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="G2">
         <v>300</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I2">
         <v>400</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>70</v>
       </c>
       <c r="K2">
         <v>500</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
         <v>68</v>
       </c>
       <c r="M2">
         <v>600</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5">
+      <c r="N2" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="35">
         <v>700</v>
       </c>
-      <c r="P2" s="7"/>
+      <c r="P2" s="28" t="s">
+        <v>82</v>
+      </c>
       <c r="Q2">
         <v>800</v>
       </c>
@@ -1071,7 +1126,7 @@
         <f>A2+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="25"/>
       <c r="C3">
         <f>C2+1</f>
         <v>101</v>
@@ -1083,32 +1138,32 @@
         <f>E2+1</f>
         <v>201</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="7"/>
       <c r="G3">
         <f>G2+1</f>
         <v>301</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="7"/>
       <c r="I3">
         <f>I2+1</f>
         <v>401</v>
       </c>
-      <c r="J3" s="9"/>
+      <c r="J3" s="7"/>
       <c r="K3">
         <f>K2+1</f>
         <v>501</v>
       </c>
-      <c r="L3" s="28"/>
+      <c r="L3" s="8"/>
       <c r="M3">
         <f>M2+1</f>
         <v>601</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="5">
+      <c r="N3" s="28"/>
+      <c r="O3" s="35">
         <f>O2+1</f>
         <v>701</v>
       </c>
-      <c r="P3" s="6"/>
+      <c r="P3" s="28"/>
       <c r="Q3">
         <f>Q2+1</f>
         <v>801</v>
@@ -1129,7 +1184,7 @@
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="25"/>
       <c r="C4">
         <f t="shared" ref="C4:C67" si="1">C3+1</f>
         <v>102</v>
@@ -1141,32 +1196,32 @@
         <f t="shared" ref="E4:E67" si="2">E3+1</f>
         <v>202</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="7"/>
       <c r="G4">
         <f t="shared" ref="G4:G67" si="3">G3+1</f>
         <v>302</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="7"/>
       <c r="I4">
         <f t="shared" ref="I4:I67" si="4">I3+1</f>
         <v>402</v>
       </c>
-      <c r="J4" s="9"/>
+      <c r="J4" s="7"/>
       <c r="K4">
         <f t="shared" ref="K4:K67" si="5">K3+1</f>
         <v>502</v>
       </c>
-      <c r="L4" s="28"/>
+      <c r="L4" s="8"/>
       <c r="M4">
         <f t="shared" ref="M4:M67" si="6">M3+1</f>
         <v>602</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="5">
+      <c r="N4" s="28"/>
+      <c r="O4" s="35">
         <f t="shared" ref="O4:O67" si="7">O3+1</f>
         <v>702</v>
       </c>
-      <c r="P4" s="6"/>
+      <c r="P4" s="28"/>
       <c r="Q4">
         <f t="shared" ref="Q4:Q67" si="8">Q3+1</f>
         <v>802</v>
@@ -1187,7 +1242,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="25"/>
       <c r="C5">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -1199,32 +1254,32 @@
         <f t="shared" si="2"/>
         <v>203</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="7"/>
       <c r="G5">
         <f t="shared" si="3"/>
         <v>303</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="7"/>
       <c r="I5">
         <f t="shared" si="4"/>
         <v>403</v>
       </c>
-      <c r="J5" s="9"/>
+      <c r="J5" s="7"/>
       <c r="K5">
         <f t="shared" si="5"/>
         <v>503</v>
       </c>
-      <c r="L5" s="28"/>
+      <c r="L5" s="8"/>
       <c r="M5">
         <f t="shared" si="6"/>
         <v>603</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="5">
+      <c r="N5" s="28"/>
+      <c r="O5" s="35">
         <f t="shared" si="7"/>
         <v>703</v>
       </c>
-      <c r="P5" s="6"/>
+      <c r="P5" s="28"/>
       <c r="Q5">
         <f t="shared" si="8"/>
         <v>803</v>
@@ -1245,7 +1300,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="25"/>
       <c r="C6">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -1257,32 +1312,32 @@
         <f t="shared" si="2"/>
         <v>204</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="7"/>
       <c r="G6">
         <f t="shared" si="3"/>
         <v>304</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="7"/>
       <c r="I6">
         <f t="shared" si="4"/>
         <v>404</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="7"/>
       <c r="K6">
         <f t="shared" si="5"/>
         <v>504</v>
       </c>
-      <c r="L6" s="28"/>
+      <c r="L6" s="8"/>
       <c r="M6">
         <f t="shared" si="6"/>
         <v>604</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="5">
+      <c r="N6" s="28"/>
+      <c r="O6" s="35">
         <f t="shared" si="7"/>
         <v>704</v>
       </c>
-      <c r="P6" s="6"/>
+      <c r="P6" s="28"/>
       <c r="Q6">
         <f t="shared" si="8"/>
         <v>804</v>
@@ -1303,7 +1358,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C7">
@@ -1317,32 +1372,32 @@
         <f t="shared" si="2"/>
         <v>205</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="7"/>
       <c r="G7">
         <f t="shared" si="3"/>
         <v>305</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="7"/>
       <c r="I7">
         <f t="shared" si="4"/>
         <v>405</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="7"/>
       <c r="K7">
         <f t="shared" si="5"/>
         <v>505</v>
       </c>
-      <c r="L7" s="28"/>
+      <c r="L7" s="8"/>
       <c r="M7">
         <f t="shared" si="6"/>
         <v>605</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="5">
+      <c r="N7" s="28"/>
+      <c r="O7" s="35">
         <f t="shared" si="7"/>
         <v>705</v>
       </c>
-      <c r="P7" s="6"/>
+      <c r="P7" s="28"/>
       <c r="Q7">
         <f t="shared" si="8"/>
         <v>805</v>
@@ -1363,7 +1418,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="10"/>
       <c r="C8">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1375,32 +1430,32 @@
         <f t="shared" si="2"/>
         <v>206</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="7"/>
       <c r="G8">
         <f t="shared" si="3"/>
         <v>306</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="7"/>
       <c r="I8">
         <f t="shared" si="4"/>
         <v>406</v>
       </c>
-      <c r="J8" s="9"/>
+      <c r="J8" s="7"/>
       <c r="K8">
         <f t="shared" si="5"/>
         <v>506</v>
       </c>
-      <c r="L8" s="28"/>
+      <c r="L8" s="8"/>
       <c r="M8">
         <f t="shared" si="6"/>
         <v>606</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="5">
+      <c r="N8" s="28"/>
+      <c r="O8" s="35">
         <f t="shared" si="7"/>
         <v>706</v>
       </c>
-      <c r="P8" s="6"/>
+      <c r="P8" s="28"/>
       <c r="Q8">
         <f t="shared" si="8"/>
         <v>806</v>
@@ -1421,7 +1476,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="10"/>
       <c r="C9">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1433,32 +1488,32 @@
         <f t="shared" si="2"/>
         <v>207</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="7"/>
       <c r="G9">
         <f t="shared" si="3"/>
         <v>307</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="7"/>
       <c r="I9">
         <f t="shared" si="4"/>
         <v>407</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="7"/>
       <c r="K9">
         <f t="shared" si="5"/>
         <v>507</v>
       </c>
-      <c r="L9" s="28"/>
+      <c r="L9" s="8"/>
       <c r="M9">
         <f t="shared" si="6"/>
         <v>607</v>
       </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="5">
+      <c r="N9" s="28"/>
+      <c r="O9" s="35">
         <f t="shared" si="7"/>
         <v>707</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="P9" s="28"/>
       <c r="Q9">
         <f t="shared" si="8"/>
         <v>807</v>
@@ -1473,7 +1528,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="10"/>
       <c r="C10">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1485,32 +1540,32 @@
         <f t="shared" si="2"/>
         <v>208</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="7"/>
       <c r="G10">
         <f t="shared" si="3"/>
         <v>308</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="7"/>
       <c r="I10">
         <f t="shared" si="4"/>
         <v>408</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="7"/>
       <c r="K10">
         <f t="shared" si="5"/>
         <v>508</v>
       </c>
-      <c r="L10" s="28"/>
+      <c r="L10" s="8"/>
       <c r="M10">
         <f t="shared" si="6"/>
         <v>608</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="5">
+      <c r="N10" s="28"/>
+      <c r="O10" s="35">
         <f t="shared" si="7"/>
         <v>708</v>
       </c>
-      <c r="P10" s="6"/>
+      <c r="P10" s="28"/>
       <c r="Q10">
         <f t="shared" si="8"/>
         <v>808</v>
@@ -1525,7 +1580,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="10"/>
       <c r="C11">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1537,32 +1592,32 @@
         <f t="shared" si="2"/>
         <v>209</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="7"/>
       <c r="G11">
         <f t="shared" si="3"/>
         <v>309</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="7"/>
       <c r="I11">
         <f t="shared" si="4"/>
         <v>409</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="7"/>
       <c r="K11">
         <f t="shared" si="5"/>
         <v>509</v>
       </c>
-      <c r="L11" s="28"/>
+      <c r="L11" s="8"/>
       <c r="M11">
         <f t="shared" si="6"/>
         <v>609</v>
       </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="5">
+      <c r="N11" s="28"/>
+      <c r="O11" s="35">
         <f t="shared" si="7"/>
         <v>709</v>
       </c>
-      <c r="P11" s="6"/>
+      <c r="P11" s="28"/>
       <c r="Q11">
         <f t="shared" si="8"/>
         <v>809</v>
@@ -1577,7 +1632,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="10"/>
       <c r="C12">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1589,32 +1644,32 @@
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="7"/>
       <c r="G12">
         <f t="shared" si="3"/>
         <v>310</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="7"/>
       <c r="I12">
         <f t="shared" si="4"/>
         <v>410</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="7"/>
       <c r="K12">
         <f t="shared" si="5"/>
         <v>510</v>
       </c>
-      <c r="L12" s="28"/>
+      <c r="L12" s="8"/>
       <c r="M12">
         <f t="shared" si="6"/>
         <v>610</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="5">
+      <c r="N12" s="28"/>
+      <c r="O12" s="35">
         <f t="shared" si="7"/>
         <v>710</v>
       </c>
-      <c r="P12" s="6"/>
+      <c r="P12" s="28"/>
       <c r="Q12">
         <f t="shared" si="8"/>
         <v>810</v>
@@ -1629,44 +1684,44 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="10"/>
       <c r="C13">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="19" t="s">
         <v>59</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
         <v>211</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="7"/>
       <c r="G13">
         <f t="shared" si="3"/>
         <v>311</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="7"/>
       <c r="I13">
         <f t="shared" si="4"/>
         <v>411</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="7"/>
       <c r="K13">
         <f t="shared" si="5"/>
         <v>511</v>
       </c>
-      <c r="L13" s="28"/>
+      <c r="L13" s="8"/>
       <c r="M13">
         <f t="shared" si="6"/>
         <v>611</v>
       </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="5">
+      <c r="N13" s="28"/>
+      <c r="O13" s="35">
         <f t="shared" si="7"/>
         <v>711</v>
       </c>
-      <c r="P13" s="6"/>
+      <c r="P13" s="28"/>
       <c r="Q13">
         <f t="shared" si="8"/>
         <v>811</v>
@@ -1681,42 +1736,42 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="10"/>
       <c r="C14">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="20"/>
       <c r="E14">
         <f t="shared" si="2"/>
         <v>212</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="7"/>
       <c r="G14">
         <f t="shared" si="3"/>
         <v>312</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="7"/>
       <c r="I14">
         <f t="shared" si="4"/>
         <v>412</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="7"/>
       <c r="K14">
         <f t="shared" si="5"/>
         <v>512</v>
       </c>
-      <c r="L14" s="28"/>
+      <c r="L14" s="8"/>
       <c r="M14">
         <f t="shared" si="6"/>
         <v>612</v>
       </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="5">
+      <c r="N14" s="28"/>
+      <c r="O14" s="35">
         <f t="shared" si="7"/>
         <v>712</v>
       </c>
-      <c r="P14" s="6"/>
+      <c r="P14" s="28"/>
       <c r="Q14">
         <f t="shared" si="8"/>
         <v>812</v>
@@ -1731,42 +1786,42 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="10"/>
       <c r="C15">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="20"/>
       <c r="E15">
         <f t="shared" si="2"/>
         <v>213</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" s="7"/>
       <c r="G15">
         <f t="shared" si="3"/>
         <v>313</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="7"/>
       <c r="I15">
         <f t="shared" si="4"/>
         <v>413</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="7"/>
       <c r="K15">
         <f t="shared" si="5"/>
         <v>513</v>
       </c>
-      <c r="L15" s="28"/>
+      <c r="L15" s="8"/>
       <c r="M15">
         <f t="shared" si="6"/>
         <v>613</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="5">
+      <c r="N15" s="28"/>
+      <c r="O15" s="35">
         <f t="shared" si="7"/>
         <v>713</v>
       </c>
-      <c r="P15" s="6"/>
+      <c r="P15" s="28"/>
       <c r="Q15">
         <f t="shared" si="8"/>
         <v>813</v>
@@ -1781,42 +1836,42 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="10"/>
       <c r="C16">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="21"/>
       <c r="E16">
         <f t="shared" si="2"/>
         <v>214</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="7"/>
       <c r="G16">
         <f t="shared" si="3"/>
         <v>314</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="7"/>
       <c r="I16">
         <f t="shared" si="4"/>
         <v>414</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="7"/>
       <c r="K16">
         <f t="shared" si="5"/>
         <v>514</v>
       </c>
-      <c r="L16" s="28"/>
+      <c r="L16" s="8"/>
       <c r="M16">
         <f t="shared" si="6"/>
         <v>614</v>
       </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="5">
+      <c r="N16" s="28"/>
+      <c r="O16" s="35">
         <f t="shared" si="7"/>
         <v>714</v>
       </c>
-      <c r="P16" s="6"/>
+      <c r="P16" s="28"/>
       <c r="Q16">
         <f t="shared" si="8"/>
         <v>814</v>
@@ -1831,44 +1886,44 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="22"/>
+      <c r="B17" s="10"/>
       <c r="C17">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="19" t="s">
         <v>60</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
         <v>215</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" s="7"/>
       <c r="G17">
         <f t="shared" si="3"/>
         <v>315</v>
       </c>
-      <c r="H17" s="9"/>
+      <c r="H17" s="7"/>
       <c r="I17">
         <f t="shared" si="4"/>
         <v>415</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="7"/>
       <c r="K17">
         <f t="shared" si="5"/>
         <v>515</v>
       </c>
-      <c r="L17" s="28"/>
+      <c r="L17" s="8"/>
       <c r="M17">
         <f t="shared" si="6"/>
         <v>615</v>
       </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="5">
+      <c r="N17" s="29"/>
+      <c r="O17" s="35">
         <f t="shared" si="7"/>
         <v>715</v>
       </c>
-      <c r="P17" s="6"/>
+      <c r="P17" s="29"/>
       <c r="Q17">
         <f t="shared" si="8"/>
         <v>815</v>
@@ -1883,42 +1938,46 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="10"/>
       <c r="C18">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="20"/>
       <c r="E18">
         <f t="shared" si="2"/>
         <v>216</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" s="7"/>
       <c r="G18">
         <f t="shared" si="3"/>
         <v>316</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="7"/>
       <c r="I18">
         <f t="shared" si="4"/>
         <v>416</v>
       </c>
-      <c r="J18" s="9"/>
+      <c r="J18" s="7"/>
       <c r="K18">
         <f t="shared" si="5"/>
         <v>516</v>
       </c>
-      <c r="L18" s="28"/>
+      <c r="L18" s="8"/>
       <c r="M18">
         <f t="shared" si="6"/>
         <v>616</v>
       </c>
-      <c r="N18" s="6"/>
+      <c r="N18" s="27" t="s">
+        <v>80</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="7"/>
         <v>716</v>
       </c>
-      <c r="P18" s="6"/>
+      <c r="P18" s="27" t="s">
+        <v>86</v>
+      </c>
       <c r="Q18">
         <f t="shared" si="8"/>
         <v>816</v>
@@ -1933,42 +1992,42 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="10"/>
       <c r="C19">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="20"/>
       <c r="E19">
         <f t="shared" si="2"/>
         <v>217</v>
       </c>
-      <c r="F19" s="9"/>
+      <c r="F19" s="7"/>
       <c r="G19">
         <f t="shared" si="3"/>
         <v>317</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="7"/>
       <c r="I19">
         <f t="shared" si="4"/>
         <v>417</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="7"/>
       <c r="K19">
         <f t="shared" si="5"/>
         <v>517</v>
       </c>
-      <c r="L19" s="28"/>
+      <c r="L19" s="8"/>
       <c r="M19">
         <f t="shared" si="6"/>
         <v>617</v>
       </c>
-      <c r="N19" s="6"/>
+      <c r="N19" s="28"/>
       <c r="O19" s="5">
         <f t="shared" si="7"/>
         <v>717</v>
       </c>
-      <c r="P19" s="6"/>
+      <c r="P19" s="28"/>
       <c r="Q19">
         <f t="shared" si="8"/>
         <v>817</v>
@@ -1983,42 +2042,42 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="22"/>
+      <c r="B20" s="10"/>
       <c r="C20">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="D20" s="12"/>
+      <c r="D20" s="21"/>
       <c r="E20">
         <f t="shared" si="2"/>
         <v>218</v>
       </c>
-      <c r="F20" s="9"/>
+      <c r="F20" s="7"/>
       <c r="G20">
         <f t="shared" si="3"/>
         <v>318</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="7"/>
       <c r="I20">
         <f t="shared" si="4"/>
         <v>418</v>
       </c>
-      <c r="J20" s="9"/>
+      <c r="J20" s="7"/>
       <c r="K20">
         <f t="shared" si="5"/>
         <v>518</v>
       </c>
-      <c r="L20" s="28"/>
+      <c r="L20" s="8"/>
       <c r="M20">
         <f t="shared" si="6"/>
         <v>618</v>
       </c>
-      <c r="N20" s="6"/>
+      <c r="N20" s="28"/>
       <c r="O20" s="5">
         <f t="shared" si="7"/>
         <v>718</v>
       </c>
-      <c r="P20" s="6"/>
+      <c r="P20" s="28"/>
       <c r="Q20">
         <f t="shared" si="8"/>
         <v>818</v>
@@ -2033,44 +2092,44 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="10"/>
       <c r="C21">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="22" t="s">
         <v>72</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
         <v>219</v>
       </c>
-      <c r="F21" s="9"/>
+      <c r="F21" s="7"/>
       <c r="G21">
         <f t="shared" si="3"/>
         <v>319</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="7"/>
       <c r="I21">
         <f t="shared" si="4"/>
         <v>419</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="7"/>
       <c r="K21">
         <f t="shared" si="5"/>
         <v>519</v>
       </c>
-      <c r="L21" s="28"/>
+      <c r="L21" s="8"/>
       <c r="M21">
         <f t="shared" si="6"/>
         <v>619</v>
       </c>
-      <c r="N21" s="6"/>
+      <c r="N21" s="28"/>
       <c r="O21" s="5">
         <f t="shared" si="7"/>
         <v>719</v>
       </c>
-      <c r="P21" s="6"/>
+      <c r="P21" s="28"/>
       <c r="Q21">
         <f t="shared" si="8"/>
         <v>819</v>
@@ -2085,42 +2144,42 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="22"/>
+      <c r="B22" s="10"/>
       <c r="C22">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="23"/>
       <c r="E22">
         <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="F22" s="9"/>
+      <c r="F22" s="7"/>
       <c r="G22">
         <f t="shared" si="3"/>
         <v>320</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="7"/>
       <c r="I22">
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="7"/>
       <c r="K22">
         <f t="shared" si="5"/>
         <v>520</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="8"/>
       <c r="M22">
         <f t="shared" si="6"/>
         <v>620</v>
       </c>
-      <c r="N22" s="6"/>
+      <c r="N22" s="28"/>
       <c r="O22" s="5">
         <f t="shared" si="7"/>
         <v>720</v>
       </c>
-      <c r="P22" s="6"/>
+      <c r="P22" s="28"/>
       <c r="Q22">
         <f t="shared" si="8"/>
         <v>820</v>
@@ -2135,7 +2194,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="10"/>
       <c r="C23">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -2147,32 +2206,32 @@
         <f t="shared" si="2"/>
         <v>221</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="7"/>
       <c r="G23">
         <f t="shared" si="3"/>
         <v>321</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="7"/>
       <c r="I23">
         <f t="shared" si="4"/>
         <v>421</v>
       </c>
-      <c r="J23" s="9"/>
+      <c r="J23" s="7"/>
       <c r="K23">
         <f t="shared" si="5"/>
         <v>521</v>
       </c>
-      <c r="L23" s="28"/>
+      <c r="L23" s="8"/>
       <c r="M23">
         <f t="shared" si="6"/>
         <v>621</v>
       </c>
-      <c r="N23" s="6"/>
+      <c r="N23" s="28"/>
       <c r="O23" s="5">
         <f t="shared" si="7"/>
         <v>721</v>
       </c>
-      <c r="P23" s="6"/>
+      <c r="P23" s="28"/>
       <c r="Q23">
         <f t="shared" si="8"/>
         <v>821</v>
@@ -2187,7 +2246,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="22"/>
+      <c r="B24" s="10"/>
       <c r="C24">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -2199,32 +2258,32 @@
         <f t="shared" si="2"/>
         <v>222</v>
       </c>
-      <c r="F24" s="9"/>
+      <c r="F24" s="7"/>
       <c r="G24">
         <f t="shared" si="3"/>
         <v>322</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="7"/>
       <c r="I24">
         <f t="shared" si="4"/>
         <v>422</v>
       </c>
-      <c r="J24" s="9"/>
+      <c r="J24" s="7"/>
       <c r="K24">
         <f t="shared" si="5"/>
         <v>522</v>
       </c>
-      <c r="L24" s="28"/>
+      <c r="L24" s="8"/>
       <c r="M24">
         <f t="shared" si="6"/>
         <v>622</v>
       </c>
-      <c r="N24" s="6"/>
+      <c r="N24" s="28"/>
       <c r="O24" s="5">
         <f t="shared" si="7"/>
         <v>722</v>
       </c>
-      <c r="P24" s="6"/>
+      <c r="P24" s="28"/>
       <c r="Q24">
         <f t="shared" si="8"/>
         <v>822</v>
@@ -2239,7 +2298,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="22"/>
+      <c r="B25" s="10"/>
       <c r="C25">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -2251,32 +2310,32 @@
         <f t="shared" si="2"/>
         <v>223</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="7"/>
       <c r="G25">
         <f t="shared" si="3"/>
         <v>323</v>
       </c>
-      <c r="H25" s="9"/>
+      <c r="H25" s="7"/>
       <c r="I25">
         <f t="shared" si="4"/>
         <v>423</v>
       </c>
-      <c r="J25" s="9"/>
+      <c r="J25" s="7"/>
       <c r="K25">
         <f t="shared" si="5"/>
         <v>523</v>
       </c>
-      <c r="L25" s="28"/>
+      <c r="L25" s="8"/>
       <c r="M25">
         <f t="shared" si="6"/>
         <v>623</v>
       </c>
-      <c r="N25" s="6"/>
+      <c r="N25" s="28"/>
       <c r="O25" s="5">
         <f t="shared" si="7"/>
         <v>723</v>
       </c>
-      <c r="P25" s="6"/>
+      <c r="P25" s="28"/>
       <c r="Q25">
         <f t="shared" si="8"/>
         <v>823</v>
@@ -2291,44 +2350,44 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="22"/>
+      <c r="B26" s="10"/>
       <c r="C26">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
         <v>224</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="7"/>
       <c r="G26">
         <f t="shared" si="3"/>
         <v>324</v>
       </c>
-      <c r="H26" s="9"/>
+      <c r="H26" s="7"/>
       <c r="I26">
         <f t="shared" si="4"/>
         <v>424</v>
       </c>
-      <c r="J26" s="9"/>
+      <c r="J26" s="7"/>
       <c r="K26">
         <f t="shared" si="5"/>
         <v>524</v>
       </c>
-      <c r="L26" s="28"/>
+      <c r="L26" s="8"/>
       <c r="M26">
         <f t="shared" si="6"/>
         <v>624</v>
       </c>
-      <c r="N26" s="6"/>
+      <c r="N26" s="28"/>
       <c r="O26" s="5">
         <f t="shared" si="7"/>
         <v>724</v>
       </c>
-      <c r="P26" s="6"/>
+      <c r="P26" s="28"/>
       <c r="Q26">
         <f t="shared" si="8"/>
         <v>824</v>
@@ -2343,48 +2402,48 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="22"/>
+      <c r="B27" s="10"/>
       <c r="C27">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="24"/>
       <c r="E27">
         <f t="shared" si="2"/>
         <v>225</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G27">
         <f t="shared" si="3"/>
         <v>325</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="6" t="s">
         <v>58</v>
       </c>
       <c r="I27">
         <f t="shared" si="4"/>
         <v>425</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="6" t="s">
         <v>71</v>
       </c>
       <c r="K27">
         <f t="shared" si="5"/>
         <v>525</v>
       </c>
-      <c r="L27" s="28"/>
+      <c r="L27" s="8"/>
       <c r="M27">
         <f t="shared" si="6"/>
         <v>625</v>
       </c>
-      <c r="N27" s="4"/>
+      <c r="N27" s="28"/>
       <c r="O27" s="5">
         <f t="shared" si="7"/>
         <v>725</v>
       </c>
-      <c r="P27" s="4"/>
+      <c r="P27" s="28"/>
       <c r="Q27">
         <f t="shared" si="8"/>
         <v>825</v>
@@ -2399,42 +2458,42 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="9"/>
       <c r="C28">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="D28" s="19"/>
+      <c r="D28" s="24"/>
       <c r="E28">
         <f t="shared" si="2"/>
         <v>226</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="7"/>
       <c r="G28">
         <f t="shared" si="3"/>
         <v>326</v>
       </c>
-      <c r="H28" s="9"/>
+      <c r="H28" s="7"/>
       <c r="I28">
         <f t="shared" si="4"/>
         <v>426</v>
       </c>
-      <c r="J28" s="9"/>
+      <c r="J28" s="7"/>
       <c r="K28">
         <f t="shared" si="5"/>
         <v>526</v>
       </c>
-      <c r="L28" s="28"/>
+      <c r="L28" s="8"/>
       <c r="M28">
         <f t="shared" si="6"/>
         <v>626</v>
       </c>
-      <c r="N28" s="4"/>
+      <c r="N28" s="28"/>
       <c r="O28" s="5">
         <f t="shared" si="7"/>
         <v>726</v>
       </c>
-      <c r="P28" s="4"/>
+      <c r="P28" s="28"/>
       <c r="Q28">
         <f t="shared" si="8"/>
         <v>826</v>
@@ -2449,42 +2508,42 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="9"/>
       <c r="C29">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="D29" s="18"/>
+      <c r="D29" s="13"/>
       <c r="E29">
         <f t="shared" si="2"/>
         <v>227</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" s="7"/>
       <c r="G29">
         <f t="shared" si="3"/>
         <v>327</v>
       </c>
-      <c r="H29" s="9"/>
+      <c r="H29" s="7"/>
       <c r="I29">
         <f t="shared" si="4"/>
         <v>427</v>
       </c>
-      <c r="J29" s="9"/>
+      <c r="J29" s="7"/>
       <c r="K29">
         <f t="shared" si="5"/>
         <v>527</v>
       </c>
-      <c r="L29" s="28"/>
+      <c r="L29" s="8"/>
       <c r="M29">
         <f t="shared" si="6"/>
         <v>627</v>
       </c>
-      <c r="N29" s="4"/>
+      <c r="N29" s="28"/>
       <c r="O29" s="5">
         <f t="shared" si="7"/>
         <v>727</v>
       </c>
-      <c r="P29" s="4"/>
+      <c r="P29" s="28"/>
       <c r="Q29">
         <f t="shared" si="8"/>
         <v>827</v>
@@ -2499,44 +2558,44 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="9"/>
       <c r="C30">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
         <v>228</v>
       </c>
-      <c r="F30" s="9"/>
+      <c r="F30" s="7"/>
       <c r="G30">
         <f t="shared" si="3"/>
         <v>328</v>
       </c>
-      <c r="H30" s="9"/>
+      <c r="H30" s="7"/>
       <c r="I30">
         <f t="shared" si="4"/>
         <v>428</v>
       </c>
-      <c r="J30" s="9"/>
+      <c r="J30" s="7"/>
       <c r="K30">
         <f t="shared" si="5"/>
         <v>528</v>
       </c>
-      <c r="L30" s="28"/>
+      <c r="L30" s="8"/>
       <c r="M30">
         <f t="shared" si="6"/>
         <v>628</v>
       </c>
-      <c r="N30" s="4"/>
+      <c r="N30" s="28"/>
       <c r="O30" s="5">
         <f t="shared" si="7"/>
         <v>728</v>
       </c>
-      <c r="P30" s="4"/>
+      <c r="P30" s="28"/>
       <c r="Q30">
         <f t="shared" si="8"/>
         <v>828</v>
@@ -2551,42 +2610,42 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="9"/>
       <c r="C31">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="D31" s="21"/>
+      <c r="D31" s="26"/>
       <c r="E31">
         <f t="shared" si="2"/>
         <v>229</v>
       </c>
-      <c r="F31" s="9"/>
+      <c r="F31" s="7"/>
       <c r="G31">
         <f t="shared" si="3"/>
         <v>329</v>
       </c>
-      <c r="H31" s="9"/>
+      <c r="H31" s="7"/>
       <c r="I31">
         <f t="shared" si="4"/>
         <v>429</v>
       </c>
-      <c r="J31" s="9"/>
+      <c r="J31" s="7"/>
       <c r="K31">
         <f t="shared" si="5"/>
         <v>529</v>
       </c>
-      <c r="L31" s="28"/>
+      <c r="L31" s="8"/>
       <c r="M31">
         <f t="shared" si="6"/>
         <v>629</v>
       </c>
-      <c r="N31" s="4"/>
+      <c r="N31" s="28"/>
       <c r="O31" s="5">
         <f t="shared" si="7"/>
         <v>729</v>
       </c>
-      <c r="P31" s="4"/>
+      <c r="P31" s="28"/>
       <c r="Q31">
         <f t="shared" si="8"/>
         <v>829</v>
@@ -2601,42 +2660,42 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="9"/>
       <c r="C32">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="D32" s="21"/>
+      <c r="D32" s="26"/>
       <c r="E32">
         <f t="shared" si="2"/>
         <v>230</v>
       </c>
-      <c r="F32" s="9"/>
+      <c r="F32" s="7"/>
       <c r="G32">
         <f t="shared" si="3"/>
         <v>330</v>
       </c>
-      <c r="H32" s="9"/>
+      <c r="H32" s="7"/>
       <c r="I32">
         <f t="shared" si="4"/>
         <v>430</v>
       </c>
-      <c r="J32" s="9"/>
+      <c r="J32" s="7"/>
       <c r="K32">
         <f t="shared" si="5"/>
         <v>530</v>
       </c>
-      <c r="L32" s="28"/>
+      <c r="L32" s="8"/>
       <c r="M32">
         <f t="shared" si="6"/>
         <v>630</v>
       </c>
-      <c r="N32" s="4"/>
+      <c r="N32" s="28"/>
       <c r="O32" s="5">
         <f t="shared" si="7"/>
         <v>730</v>
       </c>
-      <c r="P32" s="4"/>
+      <c r="P32" s="28"/>
       <c r="Q32">
         <f t="shared" si="8"/>
         <v>830</v>
@@ -2651,42 +2710,42 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="13"/>
+      <c r="B33" s="9"/>
       <c r="C33">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
-      <c r="D33" s="21"/>
+      <c r="D33" s="26"/>
       <c r="E33">
         <f t="shared" si="2"/>
         <v>231</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="F33" s="7"/>
       <c r="G33">
         <f t="shared" si="3"/>
         <v>331</v>
       </c>
-      <c r="H33" s="9"/>
+      <c r="H33" s="7"/>
       <c r="I33">
         <f t="shared" si="4"/>
         <v>431</v>
       </c>
-      <c r="J33" s="9"/>
+      <c r="J33" s="7"/>
       <c r="K33">
         <f t="shared" si="5"/>
         <v>531</v>
       </c>
-      <c r="L33" s="28"/>
+      <c r="L33" s="8"/>
       <c r="M33">
         <f t="shared" si="6"/>
         <v>631</v>
       </c>
-      <c r="N33" s="4"/>
+      <c r="N33" s="28"/>
       <c r="O33" s="5">
         <f t="shared" si="7"/>
         <v>731</v>
       </c>
-      <c r="P33" s="4"/>
+      <c r="P33" s="37"/>
       <c r="Q33">
         <f t="shared" si="8"/>
         <v>831</v>
@@ -2701,44 +2760,46 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="13"/>
+      <c r="B34" s="9"/>
       <c r="C34">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
         <v>232</v>
       </c>
-      <c r="F34" s="9"/>
+      <c r="F34" s="7"/>
       <c r="G34">
         <f t="shared" si="3"/>
         <v>332</v>
       </c>
-      <c r="H34" s="9"/>
+      <c r="H34" s="7"/>
       <c r="I34">
         <f t="shared" si="4"/>
         <v>432</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="7"/>
       <c r="K34">
         <f t="shared" si="5"/>
         <v>532</v>
       </c>
-      <c r="L34" s="28"/>
+      <c r="L34" s="8"/>
       <c r="M34">
         <f t="shared" si="6"/>
         <v>632</v>
       </c>
-      <c r="N34" s="4"/>
+      <c r="N34" s="28"/>
       <c r="O34" s="5">
         <f t="shared" si="7"/>
         <v>732</v>
       </c>
-      <c r="P34" s="4"/>
+      <c r="P34" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="Q34">
         <f t="shared" si="8"/>
         <v>832</v>
@@ -2753,42 +2814,42 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="13"/>
+      <c r="B35" s="9"/>
       <c r="C35">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="D35" s="21"/>
+      <c r="D35" s="26"/>
       <c r="E35">
         <f t="shared" si="2"/>
         <v>233</v>
       </c>
-      <c r="F35" s="9"/>
+      <c r="F35" s="7"/>
       <c r="G35">
         <f t="shared" si="3"/>
         <v>333</v>
       </c>
-      <c r="H35" s="9"/>
+      <c r="H35" s="7"/>
       <c r="I35">
         <f t="shared" si="4"/>
         <v>433</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="7"/>
       <c r="K35">
         <f t="shared" si="5"/>
         <v>533</v>
       </c>
-      <c r="L35" s="28"/>
+      <c r="L35" s="8"/>
       <c r="M35">
         <f t="shared" si="6"/>
         <v>633</v>
       </c>
-      <c r="N35" s="4"/>
+      <c r="N35" s="28"/>
       <c r="O35" s="5">
         <f t="shared" si="7"/>
         <v>733</v>
       </c>
-      <c r="P35" s="4"/>
+      <c r="P35" s="31"/>
       <c r="Q35">
         <f t="shared" si="8"/>
         <v>833</v>
@@ -2803,42 +2864,44 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="13"/>
+      <c r="B36" s="9"/>
       <c r="C36">
         <f t="shared" si="1"/>
         <v>134</v>
       </c>
-      <c r="D36" s="21"/>
+      <c r="D36" s="26"/>
       <c r="E36">
         <f t="shared" si="2"/>
         <v>234</v>
       </c>
-      <c r="F36" s="9"/>
+      <c r="F36" s="7"/>
       <c r="G36">
         <f t="shared" si="3"/>
         <v>334</v>
       </c>
-      <c r="H36" s="9"/>
+      <c r="H36" s="7"/>
       <c r="I36">
         <f t="shared" si="4"/>
         <v>434</v>
       </c>
-      <c r="J36" s="9"/>
+      <c r="J36" s="7"/>
       <c r="K36">
         <f t="shared" si="5"/>
         <v>534</v>
       </c>
-      <c r="L36" s="28"/>
+      <c r="L36" s="8"/>
       <c r="M36">
         <f t="shared" si="6"/>
         <v>634</v>
       </c>
-      <c r="N36" s="4"/>
+      <c r="N36" s="28"/>
       <c r="O36" s="5">
         <f t="shared" si="7"/>
         <v>734</v>
       </c>
-      <c r="P36" s="4"/>
+      <c r="P36" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="Q36">
         <f t="shared" si="8"/>
         <v>834</v>
@@ -2853,42 +2916,42 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="9"/>
       <c r="C37">
         <f t="shared" si="1"/>
         <v>135</v>
       </c>
-      <c r="D37" s="21"/>
+      <c r="D37" s="26"/>
       <c r="E37">
         <f t="shared" si="2"/>
         <v>235</v>
       </c>
-      <c r="F37" s="9"/>
+      <c r="F37" s="7"/>
       <c r="G37">
         <f t="shared" si="3"/>
         <v>335</v>
       </c>
-      <c r="H37" s="9"/>
+      <c r="H37" s="7"/>
       <c r="I37">
         <f t="shared" si="4"/>
         <v>435</v>
       </c>
-      <c r="J37" s="9"/>
+      <c r="J37" s="7"/>
       <c r="K37">
         <f t="shared" si="5"/>
         <v>535</v>
       </c>
-      <c r="L37" s="28"/>
+      <c r="L37" s="8"/>
       <c r="M37">
         <f t="shared" si="6"/>
         <v>635</v>
       </c>
-      <c r="N37" s="4"/>
+      <c r="N37" s="28"/>
       <c r="O37" s="5">
         <f t="shared" si="7"/>
         <v>735</v>
       </c>
-      <c r="P37" s="4"/>
+      <c r="P37" s="28"/>
       <c r="Q37">
         <f t="shared" si="8"/>
         <v>835</v>
@@ -2903,7 +2966,7 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="9"/>
       <c r="C38">
         <f t="shared" si="1"/>
         <v>136</v>
@@ -2915,32 +2978,32 @@
         <f t="shared" si="2"/>
         <v>236</v>
       </c>
-      <c r="F38" s="9"/>
+      <c r="F38" s="7"/>
       <c r="G38">
         <f t="shared" si="3"/>
         <v>336</v>
       </c>
-      <c r="H38" s="9"/>
+      <c r="H38" s="7"/>
       <c r="I38">
         <f t="shared" si="4"/>
         <v>436</v>
       </c>
-      <c r="J38" s="9"/>
+      <c r="J38" s="7"/>
       <c r="K38">
         <f t="shared" si="5"/>
         <v>536</v>
       </c>
-      <c r="L38" s="28"/>
+      <c r="L38" s="8"/>
       <c r="M38">
         <f t="shared" si="6"/>
         <v>636</v>
       </c>
-      <c r="N38" s="4"/>
+      <c r="N38" s="28"/>
       <c r="O38" s="5">
         <f t="shared" si="7"/>
         <v>736</v>
       </c>
-      <c r="P38" s="4"/>
+      <c r="P38" s="28"/>
       <c r="Q38">
         <f t="shared" si="8"/>
         <v>836</v>
@@ -2955,7 +3018,7 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B39" s="13"/>
+      <c r="B39" s="9"/>
       <c r="C39">
         <f t="shared" si="1"/>
         <v>137</v>
@@ -2967,32 +3030,32 @@
         <f t="shared" si="2"/>
         <v>237</v>
       </c>
-      <c r="F39" s="9"/>
+      <c r="F39" s="7"/>
       <c r="G39">
         <f t="shared" si="3"/>
         <v>337</v>
       </c>
-      <c r="H39" s="9"/>
+      <c r="H39" s="7"/>
       <c r="I39">
         <f t="shared" si="4"/>
         <v>437</v>
       </c>
-      <c r="J39" s="9"/>
+      <c r="J39" s="7"/>
       <c r="K39">
         <f t="shared" si="5"/>
         <v>537</v>
       </c>
-      <c r="L39" s="28"/>
+      <c r="L39" s="8"/>
       <c r="M39">
         <f t="shared" si="6"/>
         <v>637</v>
       </c>
-      <c r="N39" s="4"/>
+      <c r="N39" s="28"/>
       <c r="O39" s="5">
         <f t="shared" si="7"/>
         <v>737</v>
       </c>
-      <c r="P39" s="4"/>
+      <c r="P39" s="28"/>
       <c r="Q39">
         <f t="shared" si="8"/>
         <v>837</v>
@@ -3007,44 +3070,44 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B40" s="13"/>
+      <c r="B40" s="9"/>
       <c r="C40">
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D40" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
         <v>238</v>
       </c>
-      <c r="F40" s="9"/>
+      <c r="F40" s="7"/>
       <c r="G40">
         <f t="shared" si="3"/>
         <v>338</v>
       </c>
-      <c r="H40" s="9"/>
+      <c r="H40" s="7"/>
       <c r="I40">
         <f t="shared" si="4"/>
         <v>438</v>
       </c>
-      <c r="J40" s="9"/>
+      <c r="J40" s="7"/>
       <c r="K40">
         <f t="shared" si="5"/>
         <v>538</v>
       </c>
-      <c r="L40" s="28"/>
+      <c r="L40" s="8"/>
       <c r="M40">
         <f t="shared" si="6"/>
         <v>638</v>
       </c>
-      <c r="N40" s="4"/>
+      <c r="N40" s="28"/>
       <c r="O40" s="5">
         <f t="shared" si="7"/>
         <v>738</v>
       </c>
-      <c r="P40" s="4"/>
+      <c r="P40" s="28"/>
       <c r="Q40">
         <f t="shared" si="8"/>
         <v>838</v>
@@ -3059,42 +3122,42 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="13"/>
+      <c r="B41" s="9"/>
       <c r="C41">
         <f t="shared" si="1"/>
         <v>139</v>
       </c>
-      <c r="D41" s="25"/>
+      <c r="D41" s="16"/>
       <c r="E41">
         <f t="shared" si="2"/>
         <v>239</v>
       </c>
-      <c r="F41" s="9"/>
+      <c r="F41" s="7"/>
       <c r="G41">
         <f t="shared" si="3"/>
         <v>339</v>
       </c>
-      <c r="H41" s="9"/>
+      <c r="H41" s="7"/>
       <c r="I41">
         <f t="shared" si="4"/>
         <v>439</v>
       </c>
-      <c r="J41" s="9"/>
+      <c r="J41" s="7"/>
       <c r="K41">
         <f t="shared" si="5"/>
         <v>539</v>
       </c>
-      <c r="L41" s="28"/>
+      <c r="L41" s="8"/>
       <c r="M41">
         <f t="shared" si="6"/>
         <v>639</v>
       </c>
-      <c r="N41" s="4"/>
+      <c r="N41" s="28"/>
       <c r="O41" s="5">
         <f t="shared" si="7"/>
         <v>739</v>
       </c>
-      <c r="P41" s="4"/>
+      <c r="P41" s="28"/>
       <c r="Q41">
         <f t="shared" si="8"/>
         <v>839</v>
@@ -3109,42 +3172,42 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" s="13"/>
+      <c r="B42" s="9"/>
       <c r="C42">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="17"/>
       <c r="E42">
         <f t="shared" si="2"/>
         <v>240</v>
       </c>
-      <c r="F42" s="9"/>
+      <c r="F42" s="7"/>
       <c r="G42">
         <f t="shared" si="3"/>
         <v>340</v>
       </c>
-      <c r="H42" s="9"/>
+      <c r="H42" s="7"/>
       <c r="I42">
         <f t="shared" si="4"/>
         <v>440</v>
       </c>
-      <c r="J42" s="9"/>
+      <c r="J42" s="7"/>
       <c r="K42">
         <f t="shared" si="5"/>
         <v>540</v>
       </c>
-      <c r="L42" s="28"/>
+      <c r="L42" s="8"/>
       <c r="M42">
         <f t="shared" si="6"/>
         <v>640</v>
       </c>
-      <c r="N42" s="4"/>
+      <c r="N42" s="28"/>
       <c r="O42" s="5">
         <f t="shared" si="7"/>
         <v>740</v>
       </c>
-      <c r="P42" s="4"/>
+      <c r="P42" s="28"/>
       <c r="Q42">
         <f t="shared" si="8"/>
         <v>840</v>
@@ -3159,42 +3222,42 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="13"/>
+      <c r="B43" s="9"/>
       <c r="C43">
         <f t="shared" si="1"/>
         <v>141</v>
       </c>
-      <c r="D43" s="27"/>
+      <c r="D43" s="18"/>
       <c r="E43">
         <f t="shared" si="2"/>
         <v>241</v>
       </c>
-      <c r="F43" s="9"/>
+      <c r="F43" s="7"/>
       <c r="G43">
         <f t="shared" si="3"/>
         <v>341</v>
       </c>
-      <c r="H43" s="9"/>
+      <c r="H43" s="7"/>
       <c r="I43">
         <f t="shared" si="4"/>
         <v>441</v>
       </c>
-      <c r="J43" s="9"/>
+      <c r="J43" s="7"/>
       <c r="K43">
         <f t="shared" si="5"/>
         <v>541</v>
       </c>
-      <c r="L43" s="28"/>
+      <c r="L43" s="8"/>
       <c r="M43">
         <f t="shared" si="6"/>
         <v>641</v>
       </c>
-      <c r="N43" s="4"/>
+      <c r="N43" s="28"/>
       <c r="O43" s="5">
         <f t="shared" si="7"/>
         <v>741</v>
       </c>
-      <c r="P43" s="4"/>
+      <c r="P43" s="28"/>
       <c r="Q43">
         <f t="shared" si="8"/>
         <v>841</v>
@@ -3209,44 +3272,44 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="13"/>
+      <c r="B44" s="9"/>
       <c r="C44">
         <f t="shared" si="1"/>
         <v>142</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E44">
         <f t="shared" si="2"/>
         <v>242</v>
       </c>
-      <c r="F44" s="9"/>
+      <c r="F44" s="7"/>
       <c r="G44">
         <f t="shared" si="3"/>
         <v>342</v>
       </c>
-      <c r="H44" s="9"/>
+      <c r="H44" s="7"/>
       <c r="I44">
         <f t="shared" si="4"/>
         <v>442</v>
       </c>
-      <c r="J44" s="9"/>
+      <c r="J44" s="7"/>
       <c r="K44">
         <f t="shared" si="5"/>
         <v>542</v>
       </c>
-      <c r="L44" s="28"/>
+      <c r="L44" s="8"/>
       <c r="M44">
         <f t="shared" si="6"/>
         <v>642</v>
       </c>
-      <c r="N44" s="4"/>
+      <c r="N44" s="28"/>
       <c r="O44" s="5">
         <f t="shared" si="7"/>
         <v>742</v>
       </c>
-      <c r="P44" s="4"/>
+      <c r="P44" s="28"/>
       <c r="Q44">
         <f t="shared" si="8"/>
         <v>842</v>
@@ -3261,42 +3324,42 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B45" s="13"/>
+      <c r="B45" s="9"/>
       <c r="C45">
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
-      <c r="D45" s="23"/>
+      <c r="D45" s="14"/>
       <c r="E45">
         <f t="shared" si="2"/>
         <v>243</v>
       </c>
-      <c r="F45" s="9"/>
+      <c r="F45" s="7"/>
       <c r="G45">
         <f t="shared" si="3"/>
         <v>343</v>
       </c>
-      <c r="H45" s="9"/>
+      <c r="H45" s="7"/>
       <c r="I45">
         <f t="shared" si="4"/>
         <v>443</v>
       </c>
-      <c r="J45" s="9"/>
+      <c r="J45" s="7"/>
       <c r="K45">
         <f t="shared" si="5"/>
         <v>543</v>
       </c>
-      <c r="L45" s="28"/>
+      <c r="L45" s="8"/>
       <c r="M45">
         <f t="shared" si="6"/>
         <v>643</v>
       </c>
-      <c r="N45" s="4"/>
+      <c r="N45" s="28"/>
       <c r="O45" s="5">
         <f t="shared" si="7"/>
         <v>743</v>
       </c>
-      <c r="P45" s="4"/>
+      <c r="P45" s="28"/>
       <c r="Q45">
         <f t="shared" si="8"/>
         <v>843</v>
@@ -3311,44 +3374,44 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
         <v>144</v>
       </c>
-      <c r="D46" s="23"/>
+      <c r="D46" s="14"/>
       <c r="E46">
         <f t="shared" si="2"/>
         <v>244</v>
       </c>
-      <c r="F46" s="9"/>
+      <c r="F46" s="7"/>
       <c r="G46">
         <f t="shared" si="3"/>
         <v>344</v>
       </c>
-      <c r="H46" s="9"/>
+      <c r="H46" s="7"/>
       <c r="I46">
         <f t="shared" si="4"/>
         <v>444</v>
       </c>
-      <c r="J46" s="9"/>
+      <c r="J46" s="7"/>
       <c r="K46">
         <f t="shared" si="5"/>
         <v>544</v>
       </c>
-      <c r="L46" s="28"/>
+      <c r="L46" s="8"/>
       <c r="M46">
         <f t="shared" si="6"/>
         <v>644</v>
       </c>
-      <c r="N46" s="4"/>
+      <c r="N46" s="28"/>
       <c r="O46" s="5">
         <f t="shared" si="7"/>
         <v>744</v>
       </c>
-      <c r="P46" s="4"/>
+      <c r="P46" s="29"/>
       <c r="Q46">
         <f t="shared" si="8"/>
         <v>844</v>
@@ -3363,42 +3426,44 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="6"/>
       <c r="C47">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="D47" s="23"/>
+      <c r="D47" s="14"/>
       <c r="E47">
         <f t="shared" si="2"/>
         <v>245</v>
       </c>
-      <c r="F47" s="9"/>
+      <c r="F47" s="7"/>
       <c r="G47">
         <f t="shared" si="3"/>
         <v>345</v>
       </c>
-      <c r="H47" s="9"/>
+      <c r="H47" s="7"/>
       <c r="I47">
         <f t="shared" si="4"/>
         <v>445</v>
       </c>
-      <c r="J47" s="9"/>
+      <c r="J47" s="7"/>
       <c r="K47">
         <f t="shared" si="5"/>
         <v>545</v>
       </c>
-      <c r="L47" s="28"/>
+      <c r="L47" s="8"/>
       <c r="M47">
         <f t="shared" si="6"/>
         <v>645</v>
       </c>
-      <c r="N47" s="4"/>
+      <c r="N47" s="28"/>
       <c r="O47" s="5">
         <f t="shared" si="7"/>
         <v>745</v>
       </c>
-      <c r="P47" s="4"/>
+      <c r="P47" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="Q47">
         <f t="shared" si="8"/>
         <v>845</v>
@@ -3413,44 +3478,44 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="6"/>
       <c r="C48">
         <f t="shared" si="1"/>
         <v>146</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="D48" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
         <v>246</v>
       </c>
-      <c r="F48" s="9"/>
+      <c r="F48" s="7"/>
       <c r="G48">
         <f t="shared" si="3"/>
         <v>346</v>
       </c>
-      <c r="H48" s="9"/>
+      <c r="H48" s="7"/>
       <c r="I48">
         <f t="shared" si="4"/>
         <v>446</v>
       </c>
-      <c r="J48" s="9"/>
+      <c r="J48" s="7"/>
       <c r="K48">
         <f t="shared" si="5"/>
         <v>546</v>
       </c>
-      <c r="L48" s="28"/>
+      <c r="L48" s="8"/>
       <c r="M48">
         <f t="shared" si="6"/>
         <v>646</v>
       </c>
-      <c r="N48" s="4"/>
+      <c r="N48" s="28"/>
       <c r="O48" s="5">
         <f t="shared" si="7"/>
         <v>746</v>
       </c>
-      <c r="P48" s="4"/>
+      <c r="P48" s="28"/>
       <c r="Q48">
         <f t="shared" si="8"/>
         <v>846</v>
@@ -3465,42 +3530,42 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="6"/>
       <c r="C49">
         <f t="shared" si="1"/>
         <v>147</v>
       </c>
-      <c r="D49" s="23"/>
+      <c r="D49" s="14"/>
       <c r="E49">
         <f t="shared" si="2"/>
         <v>247</v>
       </c>
-      <c r="F49" s="9"/>
+      <c r="F49" s="7"/>
       <c r="G49">
         <f t="shared" si="3"/>
         <v>347</v>
       </c>
-      <c r="H49" s="9"/>
+      <c r="H49" s="7"/>
       <c r="I49">
         <f t="shared" si="4"/>
         <v>447</v>
       </c>
-      <c r="J49" s="9"/>
+      <c r="J49" s="7"/>
       <c r="K49">
         <f t="shared" si="5"/>
         <v>547</v>
       </c>
-      <c r="L49" s="28"/>
+      <c r="L49" s="8"/>
       <c r="M49">
         <f t="shared" si="6"/>
         <v>647</v>
       </c>
-      <c r="N49" s="4"/>
+      <c r="N49" s="28"/>
       <c r="O49" s="5">
         <f t="shared" si="7"/>
         <v>747</v>
       </c>
-      <c r="P49" s="4"/>
+      <c r="P49" s="28"/>
       <c r="Q49">
         <f t="shared" si="8"/>
         <v>847</v>
@@ -3515,42 +3580,42 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="6"/>
       <c r="C50">
         <f t="shared" si="1"/>
         <v>148</v>
       </c>
-      <c r="D50" s="23"/>
+      <c r="D50" s="14"/>
       <c r="E50">
         <f t="shared" si="2"/>
         <v>248</v>
       </c>
-      <c r="F50" s="9"/>
+      <c r="F50" s="7"/>
       <c r="G50">
         <f t="shared" si="3"/>
         <v>348</v>
       </c>
-      <c r="H50" s="9"/>
+      <c r="H50" s="7"/>
       <c r="I50">
         <f t="shared" si="4"/>
         <v>448</v>
       </c>
-      <c r="J50" s="9"/>
+      <c r="J50" s="7"/>
       <c r="K50">
         <f t="shared" si="5"/>
         <v>548</v>
       </c>
-      <c r="L50" s="28"/>
+      <c r="L50" s="8"/>
       <c r="M50">
         <f t="shared" si="6"/>
         <v>648</v>
       </c>
-      <c r="N50" s="4"/>
+      <c r="N50" s="28"/>
       <c r="O50" s="5">
         <f t="shared" si="7"/>
         <v>748</v>
       </c>
-      <c r="P50" s="4"/>
+      <c r="P50" s="28"/>
       <c r="Q50">
         <f t="shared" si="8"/>
         <v>848</v>
@@ -3565,42 +3630,42 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="6"/>
       <c r="C51">
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-      <c r="D51" s="23"/>
+      <c r="D51" s="14"/>
       <c r="E51">
         <f t="shared" si="2"/>
         <v>249</v>
       </c>
-      <c r="F51" s="9"/>
+      <c r="F51" s="7"/>
       <c r="G51">
         <f t="shared" si="3"/>
         <v>349</v>
       </c>
-      <c r="H51" s="9"/>
+      <c r="H51" s="7"/>
       <c r="I51">
         <f t="shared" si="4"/>
         <v>449</v>
       </c>
-      <c r="J51" s="9"/>
+      <c r="J51" s="7"/>
       <c r="K51">
         <f t="shared" si="5"/>
         <v>549</v>
       </c>
-      <c r="L51" s="28"/>
+      <c r="L51" s="8"/>
       <c r="M51">
         <f t="shared" si="6"/>
         <v>649</v>
       </c>
-      <c r="N51" s="4"/>
+      <c r="N51" s="28"/>
       <c r="O51" s="5">
         <f t="shared" si="7"/>
         <v>749</v>
       </c>
-      <c r="P51" s="4"/>
+      <c r="P51" s="28"/>
       <c r="Q51">
         <f t="shared" si="8"/>
         <v>849</v>
@@ -3615,7 +3680,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="6"/>
       <c r="C52">
         <f t="shared" si="1"/>
         <v>150</v>
@@ -3627,40 +3692,40 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G52">
         <f t="shared" si="3"/>
         <v>350</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" s="6" t="s">
         <v>66</v>
       </c>
       <c r="I52">
         <f t="shared" si="4"/>
         <v>450</v>
       </c>
-      <c r="J52" s="8" t="s">
+      <c r="J52" s="6" t="s">
         <v>67</v>
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
         <v>550</v>
       </c>
-      <c r="L52" s="8" t="s">
+      <c r="L52" s="6" t="s">
         <v>69</v>
       </c>
       <c r="M52">
         <f t="shared" si="6"/>
         <v>650</v>
       </c>
-      <c r="N52" s="4"/>
+      <c r="N52" s="28"/>
       <c r="O52" s="5">
         <f t="shared" si="7"/>
         <v>750</v>
       </c>
-      <c r="P52" s="4"/>
+      <c r="P52" s="28"/>
       <c r="Q52">
         <f t="shared" si="8"/>
         <v>850</v>
@@ -3675,7 +3740,7 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="6"/>
       <c r="C53">
         <f t="shared" si="1"/>
         <v>151</v>
@@ -3687,32 +3752,32 @@
         <f t="shared" si="2"/>
         <v>251</v>
       </c>
-      <c r="F53" s="9"/>
+      <c r="F53" s="7"/>
       <c r="G53">
         <f t="shared" si="3"/>
         <v>351</v>
       </c>
-      <c r="H53" s="9"/>
+      <c r="H53" s="7"/>
       <c r="I53">
         <f t="shared" si="4"/>
         <v>451</v>
       </c>
-      <c r="J53" s="28"/>
+      <c r="J53" s="8"/>
       <c r="K53">
         <f t="shared" si="5"/>
         <v>551</v>
       </c>
-      <c r="L53" s="28"/>
+      <c r="L53" s="8"/>
       <c r="M53">
         <f t="shared" si="6"/>
         <v>651</v>
       </c>
-      <c r="N53" s="4"/>
+      <c r="N53" s="28"/>
       <c r="O53" s="5">
         <f t="shared" si="7"/>
         <v>751</v>
       </c>
-      <c r="P53" s="4"/>
+      <c r="P53" s="28"/>
       <c r="Q53">
         <f t="shared" si="8"/>
         <v>851</v>
@@ -3727,44 +3792,44 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="6"/>
       <c r="C54">
         <f t="shared" si="1"/>
         <v>152</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E54">
         <f t="shared" si="2"/>
         <v>252</v>
       </c>
-      <c r="F54" s="9"/>
+      <c r="F54" s="7"/>
       <c r="G54">
         <f t="shared" si="3"/>
         <v>352</v>
       </c>
-      <c r="H54" s="9"/>
+      <c r="H54" s="7"/>
       <c r="I54">
         <f t="shared" si="4"/>
         <v>452</v>
       </c>
-      <c r="J54" s="28"/>
+      <c r="J54" s="8"/>
       <c r="K54">
         <f t="shared" si="5"/>
         <v>552</v>
       </c>
-      <c r="L54" s="28"/>
+      <c r="L54" s="8"/>
       <c r="M54">
         <f t="shared" si="6"/>
         <v>652</v>
       </c>
-      <c r="N54" s="4"/>
+      <c r="N54" s="28"/>
       <c r="O54" s="5">
         <f t="shared" si="7"/>
         <v>752</v>
       </c>
-      <c r="P54" s="4"/>
+      <c r="P54" s="28"/>
       <c r="Q54">
         <f t="shared" si="8"/>
         <v>852</v>
@@ -3779,42 +3844,42 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="6"/>
       <c r="C55">
         <f t="shared" si="1"/>
         <v>153</v>
       </c>
-      <c r="D55" s="19"/>
+      <c r="D55" s="24"/>
       <c r="E55">
         <f t="shared" si="2"/>
         <v>253</v>
       </c>
-      <c r="F55" s="9"/>
+      <c r="F55" s="7"/>
       <c r="G55">
         <f t="shared" si="3"/>
         <v>353</v>
       </c>
-      <c r="H55" s="9"/>
+      <c r="H55" s="7"/>
       <c r="I55">
         <f t="shared" si="4"/>
         <v>453</v>
       </c>
-      <c r="J55" s="28"/>
+      <c r="J55" s="8"/>
       <c r="K55">
         <f t="shared" si="5"/>
         <v>553</v>
       </c>
-      <c r="L55" s="28"/>
+      <c r="L55" s="8"/>
       <c r="M55">
         <f t="shared" si="6"/>
         <v>653</v>
       </c>
-      <c r="N55" s="4"/>
+      <c r="N55" s="28"/>
       <c r="O55" s="5">
         <f t="shared" si="7"/>
         <v>753</v>
       </c>
-      <c r="P55" s="4"/>
+      <c r="P55" s="28"/>
       <c r="Q55">
         <f t="shared" si="8"/>
         <v>853</v>
@@ -3829,42 +3894,42 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B56" s="8"/>
+      <c r="B56" s="6"/>
       <c r="C56">
         <f t="shared" si="1"/>
         <v>154</v>
       </c>
-      <c r="D56" s="19"/>
+      <c r="D56" s="24"/>
       <c r="E56">
         <f t="shared" si="2"/>
         <v>254</v>
       </c>
-      <c r="F56" s="9"/>
+      <c r="F56" s="7"/>
       <c r="G56">
         <f t="shared" si="3"/>
         <v>354</v>
       </c>
-      <c r="H56" s="9"/>
+      <c r="H56" s="7"/>
       <c r="I56">
         <f t="shared" si="4"/>
         <v>454</v>
       </c>
-      <c r="J56" s="28"/>
+      <c r="J56" s="8"/>
       <c r="K56">
         <f t="shared" si="5"/>
         <v>554</v>
       </c>
-      <c r="L56" s="28"/>
+      <c r="L56" s="8"/>
       <c r="M56">
         <f t="shared" si="6"/>
         <v>654</v>
       </c>
-      <c r="N56" s="4"/>
+      <c r="N56" s="28"/>
       <c r="O56" s="5">
         <f t="shared" si="7"/>
         <v>754</v>
       </c>
-      <c r="P56" s="4"/>
+      <c r="P56" s="28"/>
       <c r="Q56">
         <f t="shared" si="8"/>
         <v>854</v>
@@ -3879,42 +3944,42 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="6"/>
       <c r="C57">
         <f t="shared" si="1"/>
         <v>155</v>
       </c>
-      <c r="D57" s="18"/>
+      <c r="D57" s="13"/>
       <c r="E57">
         <f t="shared" si="2"/>
         <v>255</v>
       </c>
-      <c r="F57" s="9"/>
+      <c r="F57" s="7"/>
       <c r="G57">
         <f t="shared" si="3"/>
         <v>355</v>
       </c>
-      <c r="H57" s="9"/>
+      <c r="H57" s="7"/>
       <c r="I57">
         <f t="shared" si="4"/>
         <v>455</v>
       </c>
-      <c r="J57" s="28"/>
+      <c r="J57" s="8"/>
       <c r="K57">
         <f t="shared" si="5"/>
         <v>555</v>
       </c>
-      <c r="L57" s="28"/>
+      <c r="L57" s="8"/>
       <c r="M57">
         <f t="shared" si="6"/>
         <v>655</v>
       </c>
-      <c r="N57" s="4"/>
+      <c r="N57" s="28"/>
       <c r="O57" s="5">
         <f t="shared" si="7"/>
         <v>755</v>
       </c>
-      <c r="P57" s="4"/>
+      <c r="P57" s="29"/>
       <c r="Q57">
         <f t="shared" si="8"/>
         <v>855</v>
@@ -3929,39 +3994,39 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B58" s="8"/>
+      <c r="B58" s="6"/>
       <c r="C58">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E58">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="F58" s="9"/>
+      <c r="F58" s="7"/>
       <c r="G58">
         <f t="shared" si="3"/>
         <v>356</v>
       </c>
-      <c r="H58" s="9"/>
+      <c r="H58" s="7"/>
       <c r="I58">
         <f t="shared" si="4"/>
         <v>456</v>
       </c>
-      <c r="J58" s="28"/>
+      <c r="J58" s="8"/>
       <c r="K58">
         <f t="shared" si="5"/>
         <v>556</v>
       </c>
-      <c r="L58" s="28"/>
+      <c r="L58" s="8"/>
       <c r="M58">
         <f t="shared" si="6"/>
         <v>656</v>
       </c>
-      <c r="N58" s="4"/>
+      <c r="N58" s="28"/>
       <c r="O58" s="5">
         <f t="shared" si="7"/>
         <v>756</v>
@@ -3981,37 +4046,37 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B59" s="8"/>
+      <c r="B59" s="6"/>
       <c r="C59">
         <f t="shared" si="1"/>
         <v>157</v>
       </c>
-      <c r="D59" s="26"/>
+      <c r="D59" s="17"/>
       <c r="E59">
         <f t="shared" si="2"/>
         <v>257</v>
       </c>
-      <c r="F59" s="9"/>
+      <c r="F59" s="7"/>
       <c r="G59">
         <f t="shared" si="3"/>
         <v>357</v>
       </c>
-      <c r="H59" s="9"/>
+      <c r="H59" s="7"/>
       <c r="I59">
         <f t="shared" si="4"/>
         <v>457</v>
       </c>
-      <c r="J59" s="28"/>
+      <c r="J59" s="8"/>
       <c r="K59">
         <f t="shared" si="5"/>
         <v>557</v>
       </c>
-      <c r="L59" s="28"/>
+      <c r="L59" s="8"/>
       <c r="M59">
         <f t="shared" si="6"/>
         <v>657</v>
       </c>
-      <c r="N59" s="4"/>
+      <c r="N59" s="28"/>
       <c r="O59" s="5">
         <f t="shared" si="7"/>
         <v>757</v>
@@ -4031,37 +4096,37 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B60" s="8"/>
+      <c r="B60" s="6"/>
       <c r="C60">
         <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="D60" s="26"/>
+      <c r="D60" s="17"/>
       <c r="E60">
         <f t="shared" si="2"/>
         <v>258</v>
       </c>
-      <c r="F60" s="9"/>
+      <c r="F60" s="7"/>
       <c r="G60">
         <f t="shared" si="3"/>
         <v>358</v>
       </c>
-      <c r="H60" s="9"/>
+      <c r="H60" s="7"/>
       <c r="I60">
         <f t="shared" si="4"/>
         <v>458</v>
       </c>
-      <c r="J60" s="28"/>
+      <c r="J60" s="8"/>
       <c r="K60">
         <f t="shared" si="5"/>
         <v>558</v>
       </c>
-      <c r="L60" s="28"/>
+      <c r="L60" s="8"/>
       <c r="M60">
         <f t="shared" si="6"/>
         <v>658</v>
       </c>
-      <c r="N60" s="4"/>
+      <c r="N60" s="28"/>
       <c r="O60" s="5">
         <f t="shared" si="7"/>
         <v>758</v>
@@ -4081,37 +4146,37 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="6"/>
       <c r="C61">
         <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="D61" s="27"/>
+      <c r="D61" s="18"/>
       <c r="E61">
         <f t="shared" si="2"/>
         <v>259</v>
       </c>
-      <c r="F61" s="9"/>
+      <c r="F61" s="7"/>
       <c r="G61">
         <f t="shared" si="3"/>
         <v>359</v>
       </c>
-      <c r="H61" s="9"/>
+      <c r="H61" s="7"/>
       <c r="I61">
         <f t="shared" si="4"/>
         <v>459</v>
       </c>
-      <c r="J61" s="28"/>
+      <c r="J61" s="8"/>
       <c r="K61">
         <f t="shared" si="5"/>
         <v>559</v>
       </c>
-      <c r="L61" s="28"/>
+      <c r="L61" s="8"/>
       <c r="M61">
         <f t="shared" si="6"/>
         <v>659</v>
       </c>
-      <c r="N61" s="4"/>
+      <c r="N61" s="28"/>
       <c r="O61" s="5">
         <f t="shared" si="7"/>
         <v>759</v>
@@ -4131,39 +4196,39 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="8"/>
+      <c r="B62" s="6"/>
       <c r="C62">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E62">
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="F62" s="9"/>
+      <c r="F62" s="7"/>
       <c r="G62">
         <f t="shared" si="3"/>
         <v>360</v>
       </c>
-      <c r="H62" s="9"/>
+      <c r="H62" s="7"/>
       <c r="I62">
         <f t="shared" si="4"/>
         <v>460</v>
       </c>
-      <c r="J62" s="28"/>
+      <c r="J62" s="8"/>
       <c r="K62">
         <f t="shared" si="5"/>
         <v>560</v>
       </c>
-      <c r="L62" s="28"/>
+      <c r="L62" s="8"/>
       <c r="M62">
         <f t="shared" si="6"/>
         <v>660</v>
       </c>
-      <c r="N62" s="4"/>
+      <c r="N62" s="28"/>
       <c r="O62" s="5">
         <f t="shared" si="7"/>
         <v>760</v>
@@ -4183,37 +4248,37 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="8"/>
+      <c r="B63" s="6"/>
       <c r="C63">
         <f t="shared" si="1"/>
         <v>161</v>
       </c>
-      <c r="D63" s="17"/>
+      <c r="D63" s="12"/>
       <c r="E63">
         <f t="shared" si="2"/>
         <v>261</v>
       </c>
-      <c r="F63" s="9"/>
+      <c r="F63" s="7"/>
       <c r="G63">
         <f t="shared" si="3"/>
         <v>361</v>
       </c>
-      <c r="H63" s="9"/>
+      <c r="H63" s="7"/>
       <c r="I63">
         <f t="shared" si="4"/>
         <v>461</v>
       </c>
-      <c r="J63" s="28"/>
+      <c r="J63" s="8"/>
       <c r="K63">
         <f t="shared" si="5"/>
         <v>561</v>
       </c>
-      <c r="L63" s="28"/>
+      <c r="L63" s="8"/>
       <c r="M63">
         <f t="shared" si="6"/>
         <v>661</v>
       </c>
-      <c r="N63" s="4"/>
+      <c r="N63" s="28"/>
       <c r="O63" s="5">
         <f t="shared" si="7"/>
         <v>761</v>
@@ -4233,37 +4298,37 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="8"/>
+      <c r="B64" s="6"/>
       <c r="C64">
         <f t="shared" si="1"/>
         <v>162</v>
       </c>
-      <c r="D64" s="17"/>
+      <c r="D64" s="12"/>
       <c r="E64">
         <f t="shared" si="2"/>
         <v>262</v>
       </c>
-      <c r="F64" s="9"/>
+      <c r="F64" s="7"/>
       <c r="G64">
         <f t="shared" si="3"/>
         <v>362</v>
       </c>
-      <c r="H64" s="9"/>
+      <c r="H64" s="7"/>
       <c r="I64">
         <f t="shared" si="4"/>
         <v>462</v>
       </c>
-      <c r="J64" s="28"/>
+      <c r="J64" s="8"/>
       <c r="K64">
         <f t="shared" si="5"/>
         <v>562</v>
       </c>
-      <c r="L64" s="28"/>
+      <c r="L64" s="8"/>
       <c r="M64">
         <f t="shared" si="6"/>
         <v>662</v>
       </c>
-      <c r="N64" s="4"/>
+      <c r="N64" s="28"/>
       <c r="O64" s="5">
         <f t="shared" si="7"/>
         <v>762</v>
@@ -4283,37 +4348,37 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="8"/>
+      <c r="B65" s="6"/>
       <c r="C65">
         <f t="shared" si="1"/>
         <v>163</v>
       </c>
-      <c r="D65" s="18"/>
+      <c r="D65" s="13"/>
       <c r="E65">
         <f t="shared" si="2"/>
         <v>263</v>
       </c>
-      <c r="F65" s="9"/>
+      <c r="F65" s="7"/>
       <c r="G65">
         <f t="shared" si="3"/>
         <v>363</v>
       </c>
-      <c r="H65" s="9"/>
+      <c r="H65" s="7"/>
       <c r="I65">
         <f t="shared" si="4"/>
         <v>463</v>
       </c>
-      <c r="J65" s="28"/>
+      <c r="J65" s="8"/>
       <c r="K65">
         <f t="shared" si="5"/>
         <v>563</v>
       </c>
-      <c r="L65" s="28"/>
+      <c r="L65" s="8"/>
       <c r="M65">
         <f t="shared" si="6"/>
         <v>663</v>
       </c>
-      <c r="N65" s="4"/>
+      <c r="N65" s="28"/>
       <c r="O65" s="5">
         <f t="shared" si="7"/>
         <v>763</v>
@@ -4333,7 +4398,7 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="8"/>
+      <c r="B66" s="6"/>
       <c r="C66">
         <f t="shared" si="1"/>
         <v>164</v>
@@ -4345,27 +4410,27 @@
         <f t="shared" si="2"/>
         <v>264</v>
       </c>
-      <c r="F66" s="9"/>
+      <c r="F66" s="7"/>
       <c r="G66">
         <f t="shared" si="3"/>
         <v>364</v>
       </c>
-      <c r="H66" s="9"/>
+      <c r="H66" s="7"/>
       <c r="I66">
         <f t="shared" si="4"/>
         <v>464</v>
       </c>
-      <c r="J66" s="28"/>
+      <c r="J66" s="8"/>
       <c r="K66">
         <f t="shared" si="5"/>
         <v>564</v>
       </c>
-      <c r="L66" s="28"/>
+      <c r="L66" s="8"/>
       <c r="M66">
         <f t="shared" si="6"/>
         <v>664</v>
       </c>
-      <c r="N66" s="4"/>
+      <c r="N66" s="28"/>
       <c r="O66" s="5">
         <f t="shared" si="7"/>
         <v>764</v>
@@ -4385,7 +4450,7 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="8"/>
+      <c r="B67" s="6"/>
       <c r="C67">
         <f t="shared" si="1"/>
         <v>165</v>
@@ -4397,27 +4462,27 @@
         <f t="shared" si="2"/>
         <v>265</v>
       </c>
-      <c r="F67" s="9"/>
+      <c r="F67" s="7"/>
       <c r="G67">
         <f t="shared" si="3"/>
         <v>365</v>
       </c>
-      <c r="H67" s="9"/>
+      <c r="H67" s="7"/>
       <c r="I67">
         <f t="shared" si="4"/>
         <v>465</v>
       </c>
-      <c r="J67" s="28"/>
+      <c r="J67" s="8"/>
       <c r="K67">
         <f t="shared" si="5"/>
         <v>565</v>
       </c>
-      <c r="L67" s="28"/>
+      <c r="L67" s="8"/>
       <c r="M67">
         <f t="shared" si="6"/>
         <v>665</v>
       </c>
-      <c r="N67" s="4"/>
+      <c r="N67" s="29"/>
       <c r="O67" s="5">
         <f t="shared" si="7"/>
         <v>765</v>
@@ -4437,7 +4502,7 @@
         <f t="shared" ref="A68:A101" si="10">A67+1</f>
         <v>66</v>
       </c>
-      <c r="B68" s="8"/>
+      <c r="B68" s="6"/>
       <c r="C68">
         <f t="shared" ref="C68:C101" si="11">C67+1</f>
         <v>166</v>
@@ -4449,27 +4514,29 @@
         <f t="shared" ref="E68:E101" si="12">E67+1</f>
         <v>266</v>
       </c>
-      <c r="F68" s="9"/>
+      <c r="F68" s="7"/>
       <c r="G68">
         <f t="shared" ref="G68:G101" si="13">G67+1</f>
         <v>366</v>
       </c>
-      <c r="H68" s="9"/>
+      <c r="H68" s="7"/>
       <c r="I68">
         <f t="shared" ref="I68:I101" si="14">I67+1</f>
         <v>466</v>
       </c>
-      <c r="J68" s="28"/>
+      <c r="J68" s="8"/>
       <c r="K68">
         <f t="shared" ref="K68:K101" si="15">K67+1</f>
         <v>566</v>
       </c>
-      <c r="L68" s="28"/>
+      <c r="L68" s="8"/>
       <c r="M68">
         <f t="shared" ref="M68:M101" si="16">M67+1</f>
         <v>666</v>
       </c>
-      <c r="N68" s="4"/>
+      <c r="N68" s="32" t="s">
+        <v>81</v>
+      </c>
       <c r="O68" s="5">
         <f t="shared" ref="O68:O101" si="17">O67+1</f>
         <v>766</v>
@@ -4489,7 +4556,7 @@
         <f t="shared" si="10"/>
         <v>67</v>
       </c>
-      <c r="B69" s="8"/>
+      <c r="B69" s="6"/>
       <c r="C69">
         <f t="shared" si="11"/>
         <v>167</v>
@@ -4501,27 +4568,27 @@
         <f t="shared" si="12"/>
         <v>267</v>
       </c>
-      <c r="F69" s="9"/>
+      <c r="F69" s="7"/>
       <c r="G69">
         <f t="shared" si="13"/>
         <v>367</v>
       </c>
-      <c r="H69" s="9"/>
+      <c r="H69" s="7"/>
       <c r="I69">
         <f t="shared" si="14"/>
         <v>467</v>
       </c>
-      <c r="J69" s="28"/>
+      <c r="J69" s="8"/>
       <c r="K69">
         <f t="shared" si="15"/>
         <v>567</v>
       </c>
-      <c r="L69" s="28"/>
+      <c r="L69" s="8"/>
       <c r="M69">
         <f t="shared" si="16"/>
         <v>667</v>
       </c>
-      <c r="N69" s="4"/>
+      <c r="N69" s="34"/>
       <c r="O69" s="5">
         <f t="shared" si="17"/>
         <v>767</v>
@@ -4541,7 +4608,7 @@
         <f t="shared" si="10"/>
         <v>68</v>
       </c>
-      <c r="B70" s="8"/>
+      <c r="B70" s="6"/>
       <c r="C70">
         <f t="shared" si="11"/>
         <v>168</v>
@@ -4553,27 +4620,27 @@
         <f t="shared" si="12"/>
         <v>268</v>
       </c>
-      <c r="F70" s="9"/>
+      <c r="F70" s="7"/>
       <c r="G70">
         <f t="shared" si="13"/>
         <v>368</v>
       </c>
-      <c r="H70" s="9"/>
+      <c r="H70" s="7"/>
       <c r="I70">
         <f t="shared" si="14"/>
         <v>468</v>
       </c>
-      <c r="J70" s="28"/>
+      <c r="J70" s="8"/>
       <c r="K70">
         <f t="shared" si="15"/>
         <v>568</v>
       </c>
-      <c r="L70" s="28"/>
+      <c r="L70" s="8"/>
       <c r="M70">
         <f t="shared" si="16"/>
         <v>668</v>
       </c>
-      <c r="N70" s="4"/>
+      <c r="N70" s="34"/>
       <c r="O70" s="5">
         <f t="shared" si="17"/>
         <v>768</v>
@@ -4593,7 +4660,7 @@
         <f t="shared" si="10"/>
         <v>69</v>
       </c>
-      <c r="B71" s="8"/>
+      <c r="B71" s="6"/>
       <c r="C71">
         <f t="shared" si="11"/>
         <v>169</v>
@@ -4605,27 +4672,27 @@
         <f t="shared" si="12"/>
         <v>269</v>
       </c>
-      <c r="F71" s="9"/>
+      <c r="F71" s="7"/>
       <c r="G71">
         <f t="shared" si="13"/>
         <v>369</v>
       </c>
-      <c r="H71" s="9"/>
+      <c r="H71" s="7"/>
       <c r="I71">
         <f t="shared" si="14"/>
         <v>469</v>
       </c>
-      <c r="J71" s="28"/>
+      <c r="J71" s="8"/>
       <c r="K71">
         <f t="shared" si="15"/>
         <v>569</v>
       </c>
-      <c r="L71" s="28"/>
+      <c r="L71" s="8"/>
       <c r="M71">
         <f t="shared" si="16"/>
         <v>669</v>
       </c>
-      <c r="N71" s="4"/>
+      <c r="N71" s="34"/>
       <c r="O71" s="5">
         <f t="shared" si="17"/>
         <v>769</v>
@@ -4645,7 +4712,7 @@
         <f t="shared" si="10"/>
         <v>70</v>
       </c>
-      <c r="B72" s="8"/>
+      <c r="B72" s="6"/>
       <c r="C72">
         <f t="shared" si="11"/>
         <v>170</v>
@@ -4657,27 +4724,27 @@
         <f t="shared" si="12"/>
         <v>270</v>
       </c>
-      <c r="F72" s="9"/>
+      <c r="F72" s="7"/>
       <c r="G72">
         <f t="shared" si="13"/>
         <v>370</v>
       </c>
-      <c r="H72" s="9"/>
+      <c r="H72" s="7"/>
       <c r="I72">
         <f t="shared" si="14"/>
         <v>470</v>
       </c>
-      <c r="J72" s="28"/>
+      <c r="J72" s="8"/>
       <c r="K72">
         <f t="shared" si="15"/>
         <v>570</v>
       </c>
-      <c r="L72" s="28"/>
+      <c r="L72" s="8"/>
       <c r="M72">
         <f t="shared" si="16"/>
         <v>670</v>
       </c>
-      <c r="N72" s="4"/>
+      <c r="N72" s="34"/>
       <c r="O72" s="5">
         <f t="shared" si="17"/>
         <v>770</v>
@@ -4697,7 +4764,7 @@
         <f t="shared" si="10"/>
         <v>71</v>
       </c>
-      <c r="B73" s="8"/>
+      <c r="B73" s="6"/>
       <c r="C73">
         <f t="shared" si="11"/>
         <v>171</v>
@@ -4709,27 +4776,27 @@
         <f t="shared" si="12"/>
         <v>271</v>
       </c>
-      <c r="F73" s="9"/>
+      <c r="F73" s="7"/>
       <c r="G73">
         <f t="shared" si="13"/>
         <v>371</v>
       </c>
-      <c r="H73" s="9"/>
+      <c r="H73" s="7"/>
       <c r="I73">
         <f t="shared" si="14"/>
         <v>471</v>
       </c>
-      <c r="J73" s="28"/>
+      <c r="J73" s="8"/>
       <c r="K73">
         <f t="shared" si="15"/>
         <v>571</v>
       </c>
-      <c r="L73" s="28"/>
+      <c r="L73" s="8"/>
       <c r="M73">
         <f t="shared" si="16"/>
         <v>671</v>
       </c>
-      <c r="N73" s="4"/>
+      <c r="N73" s="34"/>
       <c r="O73" s="5">
         <f t="shared" si="17"/>
         <v>771</v>
@@ -4749,7 +4816,7 @@
         <f t="shared" si="10"/>
         <v>72</v>
       </c>
-      <c r="B74" s="8"/>
+      <c r="B74" s="6"/>
       <c r="C74">
         <f t="shared" si="11"/>
         <v>172</v>
@@ -4761,27 +4828,27 @@
         <f t="shared" si="12"/>
         <v>272</v>
       </c>
-      <c r="F74" s="9"/>
+      <c r="F74" s="7"/>
       <c r="G74">
         <f t="shared" si="13"/>
         <v>372</v>
       </c>
-      <c r="H74" s="9"/>
+      <c r="H74" s="7"/>
       <c r="I74">
         <f t="shared" si="14"/>
         <v>472</v>
       </c>
-      <c r="J74" s="28"/>
+      <c r="J74" s="8"/>
       <c r="K74">
         <f t="shared" si="15"/>
         <v>572</v>
       </c>
-      <c r="L74" s="28"/>
+      <c r="L74" s="8"/>
       <c r="M74">
         <f t="shared" si="16"/>
         <v>672</v>
       </c>
-      <c r="N74" s="4"/>
+      <c r="N74" s="34"/>
       <c r="O74" s="5">
         <f t="shared" si="17"/>
         <v>772</v>
@@ -4801,7 +4868,7 @@
         <f t="shared" si="10"/>
         <v>73</v>
       </c>
-      <c r="B75" s="8"/>
+      <c r="B75" s="6"/>
       <c r="C75">
         <f t="shared" si="11"/>
         <v>173</v>
@@ -4813,27 +4880,27 @@
         <f t="shared" si="12"/>
         <v>273</v>
       </c>
-      <c r="F75" s="9"/>
+      <c r="F75" s="7"/>
       <c r="G75">
         <f t="shared" si="13"/>
         <v>373</v>
       </c>
-      <c r="H75" s="9"/>
+      <c r="H75" s="7"/>
       <c r="I75">
         <f t="shared" si="14"/>
         <v>473</v>
       </c>
-      <c r="J75" s="28"/>
+      <c r="J75" s="8"/>
       <c r="K75">
         <f t="shared" si="15"/>
         <v>573</v>
       </c>
-      <c r="L75" s="28"/>
+      <c r="L75" s="8"/>
       <c r="M75">
         <f t="shared" si="16"/>
         <v>673</v>
       </c>
-      <c r="N75" s="4"/>
+      <c r="N75" s="34"/>
       <c r="O75" s="5">
         <f t="shared" si="17"/>
         <v>773</v>
@@ -4853,7 +4920,7 @@
         <f t="shared" si="10"/>
         <v>74</v>
       </c>
-      <c r="B76" s="8"/>
+      <c r="B76" s="6"/>
       <c r="C76">
         <f t="shared" si="11"/>
         <v>174</v>
@@ -4865,27 +4932,27 @@
         <f t="shared" si="12"/>
         <v>274</v>
       </c>
-      <c r="F76" s="9"/>
+      <c r="F76" s="7"/>
       <c r="G76">
         <f t="shared" si="13"/>
         <v>374</v>
       </c>
-      <c r="H76" s="9"/>
+      <c r="H76" s="7"/>
       <c r="I76">
         <f t="shared" si="14"/>
         <v>474</v>
       </c>
-      <c r="J76" s="28"/>
+      <c r="J76" s="8"/>
       <c r="K76">
         <f t="shared" si="15"/>
         <v>574</v>
       </c>
-      <c r="L76" s="28"/>
+      <c r="L76" s="8"/>
       <c r="M76">
         <f t="shared" si="16"/>
         <v>674</v>
       </c>
-      <c r="N76" s="4"/>
+      <c r="N76" s="34"/>
       <c r="O76" s="5">
         <f t="shared" si="17"/>
         <v>774</v>
@@ -4905,7 +4972,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="B77" s="8"/>
+      <c r="B77" s="6"/>
       <c r="C77">
         <f t="shared" si="11"/>
         <v>175</v>
@@ -4917,31 +4984,31 @@
         <f t="shared" si="12"/>
         <v>275</v>
       </c>
-      <c r="F77" s="8" t="s">
+      <c r="F77" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G77">
         <f t="shared" si="13"/>
         <v>375</v>
       </c>
-      <c r="H77" s="8" t="s">
+      <c r="H77" s="6" t="s">
         <v>65</v>
       </c>
       <c r="I77">
         <f t="shared" si="14"/>
         <v>475</v>
       </c>
-      <c r="J77" s="28"/>
+      <c r="J77" s="8"/>
       <c r="K77">
         <f t="shared" si="15"/>
         <v>575</v>
       </c>
-      <c r="L77" s="28"/>
+      <c r="L77" s="8"/>
       <c r="M77">
         <f t="shared" si="16"/>
         <v>675</v>
       </c>
-      <c r="N77" s="4"/>
+      <c r="N77" s="34"/>
       <c r="O77" s="5">
         <f t="shared" si="17"/>
         <v>775</v>
@@ -4961,7 +5028,7 @@
         <f t="shared" si="10"/>
         <v>76</v>
       </c>
-      <c r="B78" s="8"/>
+      <c r="B78" s="6"/>
       <c r="C78">
         <f t="shared" si="11"/>
         <v>176</v>
@@ -4973,27 +5040,27 @@
         <f t="shared" si="12"/>
         <v>276</v>
       </c>
-      <c r="F78" s="9"/>
+      <c r="F78" s="7"/>
       <c r="G78">
         <f t="shared" si="13"/>
         <v>376</v>
       </c>
-      <c r="H78" s="9"/>
+      <c r="H78" s="7"/>
       <c r="I78">
         <f t="shared" si="14"/>
         <v>476</v>
       </c>
-      <c r="J78" s="28"/>
+      <c r="J78" s="8"/>
       <c r="K78">
         <f t="shared" si="15"/>
         <v>576</v>
       </c>
-      <c r="L78" s="28"/>
+      <c r="L78" s="8"/>
       <c r="M78">
         <f t="shared" si="16"/>
         <v>676</v>
       </c>
-      <c r="N78" s="4"/>
+      <c r="N78" s="34"/>
       <c r="O78" s="5">
         <f t="shared" si="17"/>
         <v>776</v>
@@ -5013,7 +5080,7 @@
         <f t="shared" si="10"/>
         <v>77</v>
       </c>
-      <c r="B79" s="8"/>
+      <c r="B79" s="6"/>
       <c r="C79">
         <f t="shared" si="11"/>
         <v>177</v>
@@ -5025,27 +5092,27 @@
         <f t="shared" si="12"/>
         <v>277</v>
       </c>
-      <c r="F79" s="9"/>
+      <c r="F79" s="7"/>
       <c r="G79">
         <f t="shared" si="13"/>
         <v>377</v>
       </c>
-      <c r="H79" s="9"/>
+      <c r="H79" s="7"/>
       <c r="I79">
         <f t="shared" si="14"/>
         <v>477</v>
       </c>
-      <c r="J79" s="28"/>
+      <c r="J79" s="8"/>
       <c r="K79">
         <f t="shared" si="15"/>
         <v>577</v>
       </c>
-      <c r="L79" s="28"/>
+      <c r="L79" s="8"/>
       <c r="M79">
         <f t="shared" si="16"/>
         <v>677</v>
       </c>
-      <c r="N79" s="4"/>
+      <c r="N79" s="34"/>
       <c r="O79" s="5">
         <f t="shared" si="17"/>
         <v>777</v>
@@ -5065,7 +5132,7 @@
         <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="B80" s="8"/>
+      <c r="B80" s="6"/>
       <c r="C80">
         <f t="shared" si="11"/>
         <v>178</v>
@@ -5077,27 +5144,27 @@
         <f t="shared" si="12"/>
         <v>278</v>
       </c>
-      <c r="F80" s="9"/>
+      <c r="F80" s="7"/>
       <c r="G80">
         <f t="shared" si="13"/>
         <v>378</v>
       </c>
-      <c r="H80" s="9"/>
+      <c r="H80" s="7"/>
       <c r="I80">
         <f t="shared" si="14"/>
         <v>478</v>
       </c>
-      <c r="J80" s="28"/>
+      <c r="J80" s="8"/>
       <c r="K80">
         <f t="shared" si="15"/>
         <v>578</v>
       </c>
-      <c r="L80" s="28"/>
+      <c r="L80" s="8"/>
       <c r="M80">
         <f t="shared" si="16"/>
         <v>678</v>
       </c>
-      <c r="N80" s="4"/>
+      <c r="N80" s="34"/>
       <c r="O80" s="5">
         <f t="shared" si="17"/>
         <v>778</v>
@@ -5117,7 +5184,7 @@
         <f t="shared" si="10"/>
         <v>79</v>
       </c>
-      <c r="B81" s="8"/>
+      <c r="B81" s="6"/>
       <c r="C81">
         <f t="shared" si="11"/>
         <v>179</v>
@@ -5129,27 +5196,27 @@
         <f t="shared" si="12"/>
         <v>279</v>
       </c>
-      <c r="F81" s="9"/>
+      <c r="F81" s="7"/>
       <c r="G81">
         <f t="shared" si="13"/>
         <v>379</v>
       </c>
-      <c r="H81" s="9"/>
+      <c r="H81" s="7"/>
       <c r="I81">
         <f t="shared" si="14"/>
         <v>479</v>
       </c>
-      <c r="J81" s="28"/>
+      <c r="J81" s="8"/>
       <c r="K81">
         <f t="shared" si="15"/>
         <v>579</v>
       </c>
-      <c r="L81" s="28"/>
+      <c r="L81" s="8"/>
       <c r="M81">
         <f t="shared" si="16"/>
         <v>679</v>
       </c>
-      <c r="N81" s="4"/>
+      <c r="N81" s="34"/>
       <c r="O81" s="5">
         <f t="shared" si="17"/>
         <v>779</v>
@@ -5169,7 +5236,7 @@
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
-      <c r="B82" s="8"/>
+      <c r="B82" s="6"/>
       <c r="C82">
         <f t="shared" si="11"/>
         <v>180</v>
@@ -5178,27 +5245,27 @@
         <f t="shared" si="12"/>
         <v>280</v>
       </c>
-      <c r="F82" s="9"/>
+      <c r="F82" s="7"/>
       <c r="G82">
         <f t="shared" si="13"/>
         <v>380</v>
       </c>
-      <c r="H82" s="9"/>
+      <c r="H82" s="7"/>
       <c r="I82">
         <f t="shared" si="14"/>
         <v>480</v>
       </c>
-      <c r="J82" s="28"/>
+      <c r="J82" s="8"/>
       <c r="K82">
         <f t="shared" si="15"/>
         <v>580</v>
       </c>
-      <c r="L82" s="28"/>
+      <c r="L82" s="8"/>
       <c r="M82">
         <f t="shared" si="16"/>
         <v>680</v>
       </c>
-      <c r="N82" s="4"/>
+      <c r="N82" s="34"/>
       <c r="O82" s="5">
         <f t="shared" si="17"/>
         <v>780</v>
@@ -5218,7 +5285,7 @@
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
-      <c r="B83" s="8"/>
+      <c r="B83" s="6"/>
       <c r="C83">
         <f t="shared" si="11"/>
         <v>181</v>
@@ -5227,27 +5294,27 @@
         <f t="shared" si="12"/>
         <v>281</v>
       </c>
-      <c r="F83" s="9"/>
+      <c r="F83" s="7"/>
       <c r="G83">
         <f t="shared" si="13"/>
         <v>381</v>
       </c>
-      <c r="H83" s="9"/>
+      <c r="H83" s="7"/>
       <c r="I83">
         <f t="shared" si="14"/>
         <v>481</v>
       </c>
-      <c r="J83" s="28"/>
+      <c r="J83" s="8"/>
       <c r="K83">
         <f t="shared" si="15"/>
         <v>581</v>
       </c>
-      <c r="L83" s="28"/>
+      <c r="L83" s="8"/>
       <c r="M83">
         <f t="shared" si="16"/>
         <v>681</v>
       </c>
-      <c r="N83" s="4"/>
+      <c r="N83" s="34"/>
       <c r="O83" s="5">
         <f t="shared" si="17"/>
         <v>781</v>
@@ -5267,7 +5334,7 @@
         <f t="shared" si="10"/>
         <v>82</v>
       </c>
-      <c r="B84" s="8"/>
+      <c r="B84" s="6"/>
       <c r="C84">
         <f t="shared" si="11"/>
         <v>182</v>
@@ -5276,27 +5343,27 @@
         <f t="shared" si="12"/>
         <v>282</v>
       </c>
-      <c r="F84" s="9"/>
+      <c r="F84" s="7"/>
       <c r="G84">
         <f t="shared" si="13"/>
         <v>382</v>
       </c>
-      <c r="H84" s="9"/>
+      <c r="H84" s="7"/>
       <c r="I84">
         <f t="shared" si="14"/>
         <v>482</v>
       </c>
-      <c r="J84" s="28"/>
+      <c r="J84" s="8"/>
       <c r="K84">
         <f t="shared" si="15"/>
         <v>582</v>
       </c>
-      <c r="L84" s="28"/>
+      <c r="L84" s="8"/>
       <c r="M84">
         <f t="shared" si="16"/>
         <v>682</v>
       </c>
-      <c r="N84" s="4"/>
+      <c r="N84" s="34"/>
       <c r="O84" s="5">
         <f t="shared" si="17"/>
         <v>782</v>
@@ -5316,7 +5383,7 @@
         <f t="shared" si="10"/>
         <v>83</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C85">
@@ -5327,27 +5394,27 @@
         <f t="shared" si="12"/>
         <v>283</v>
       </c>
-      <c r="F85" s="9"/>
+      <c r="F85" s="7"/>
       <c r="G85">
         <f t="shared" si="13"/>
         <v>383</v>
       </c>
-      <c r="H85" s="9"/>
+      <c r="H85" s="7"/>
       <c r="I85">
         <f t="shared" si="14"/>
         <v>483</v>
       </c>
-      <c r="J85" s="28"/>
+      <c r="J85" s="8"/>
       <c r="K85">
         <f t="shared" si="15"/>
         <v>583</v>
       </c>
-      <c r="L85" s="28"/>
+      <c r="L85" s="8"/>
       <c r="M85">
         <f t="shared" si="16"/>
         <v>683</v>
       </c>
-      <c r="N85" s="4"/>
+      <c r="N85" s="34"/>
       <c r="O85" s="5">
         <f t="shared" si="17"/>
         <v>783</v>
@@ -5367,7 +5434,7 @@
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
-      <c r="B86" s="17"/>
+      <c r="B86" s="12"/>
       <c r="C86">
         <f t="shared" si="11"/>
         <v>184</v>
@@ -5376,27 +5443,27 @@
         <f t="shared" si="12"/>
         <v>284</v>
       </c>
-      <c r="F86" s="9"/>
+      <c r="F86" s="7"/>
       <c r="G86">
         <f t="shared" si="13"/>
         <v>384</v>
       </c>
-      <c r="H86" s="9"/>
+      <c r="H86" s="7"/>
       <c r="I86">
         <f t="shared" si="14"/>
         <v>484</v>
       </c>
-      <c r="J86" s="28"/>
+      <c r="J86" s="8"/>
       <c r="K86">
         <f t="shared" si="15"/>
         <v>584</v>
       </c>
-      <c r="L86" s="28"/>
+      <c r="L86" s="8"/>
       <c r="M86">
         <f t="shared" si="16"/>
         <v>684</v>
       </c>
-      <c r="N86" s="4"/>
+      <c r="N86" s="34"/>
       <c r="O86" s="5">
         <f t="shared" si="17"/>
         <v>784</v>
@@ -5416,7 +5483,7 @@
         <f t="shared" si="10"/>
         <v>85</v>
       </c>
-      <c r="B87" s="17"/>
+      <c r="B87" s="12"/>
       <c r="C87">
         <f t="shared" si="11"/>
         <v>185</v>
@@ -5425,27 +5492,27 @@
         <f t="shared" si="12"/>
         <v>285</v>
       </c>
-      <c r="F87" s="9"/>
+      <c r="F87" s="7"/>
       <c r="G87">
         <f t="shared" si="13"/>
         <v>385</v>
       </c>
-      <c r="H87" s="9"/>
+      <c r="H87" s="7"/>
       <c r="I87">
         <f t="shared" si="14"/>
         <v>485</v>
       </c>
-      <c r="J87" s="28"/>
+      <c r="J87" s="8"/>
       <c r="K87">
         <f t="shared" si="15"/>
         <v>585</v>
       </c>
-      <c r="L87" s="28"/>
+      <c r="L87" s="8"/>
       <c r="M87">
         <f t="shared" si="16"/>
         <v>685</v>
       </c>
-      <c r="N87" s="4"/>
+      <c r="N87" s="34"/>
       <c r="O87" s="5">
         <f t="shared" si="17"/>
         <v>785</v>
@@ -5465,7 +5532,7 @@
         <f t="shared" si="10"/>
         <v>86</v>
       </c>
-      <c r="B88" s="18"/>
+      <c r="B88" s="13"/>
       <c r="C88">
         <f t="shared" si="11"/>
         <v>186</v>
@@ -5474,27 +5541,27 @@
         <f t="shared" si="12"/>
         <v>286</v>
       </c>
-      <c r="F88" s="9"/>
+      <c r="F88" s="7"/>
       <c r="G88">
         <f t="shared" si="13"/>
         <v>386</v>
       </c>
-      <c r="H88" s="9"/>
+      <c r="H88" s="7"/>
       <c r="I88">
         <f t="shared" si="14"/>
         <v>486</v>
       </c>
-      <c r="J88" s="28"/>
+      <c r="J88" s="8"/>
       <c r="K88">
         <f t="shared" si="15"/>
         <v>586</v>
       </c>
-      <c r="L88" s="28"/>
+      <c r="L88" s="8"/>
       <c r="M88">
         <f t="shared" si="16"/>
         <v>686</v>
       </c>
-      <c r="N88" s="4"/>
+      <c r="N88" s="34"/>
       <c r="O88" s="5">
         <f t="shared" si="17"/>
         <v>786</v>
@@ -5525,27 +5592,27 @@
         <f t="shared" si="12"/>
         <v>287</v>
       </c>
-      <c r="F89" s="9"/>
+      <c r="F89" s="7"/>
       <c r="G89">
         <f t="shared" si="13"/>
         <v>387</v>
       </c>
-      <c r="H89" s="9"/>
+      <c r="H89" s="7"/>
       <c r="I89">
         <f t="shared" si="14"/>
         <v>487</v>
       </c>
-      <c r="J89" s="28"/>
+      <c r="J89" s="8"/>
       <c r="K89">
         <f t="shared" si="15"/>
         <v>587</v>
       </c>
-      <c r="L89" s="28"/>
+      <c r="L89" s="8"/>
       <c r="M89">
         <f t="shared" si="16"/>
         <v>687</v>
       </c>
-      <c r="N89" s="4"/>
+      <c r="N89" s="34"/>
       <c r="O89" s="5">
         <f t="shared" si="17"/>
         <v>787</v>
@@ -5576,27 +5643,27 @@
         <f t="shared" si="12"/>
         <v>288</v>
       </c>
-      <c r="F90" s="9"/>
+      <c r="F90" s="7"/>
       <c r="G90">
         <f t="shared" si="13"/>
         <v>388</v>
       </c>
-      <c r="H90" s="9"/>
+      <c r="H90" s="7"/>
       <c r="I90">
         <f t="shared" si="14"/>
         <v>488</v>
       </c>
-      <c r="J90" s="28"/>
+      <c r="J90" s="8"/>
       <c r="K90">
         <f t="shared" si="15"/>
         <v>588</v>
       </c>
-      <c r="L90" s="28"/>
+      <c r="L90" s="8"/>
       <c r="M90">
         <f t="shared" si="16"/>
         <v>688</v>
       </c>
-      <c r="N90" s="4"/>
+      <c r="N90" s="34"/>
       <c r="O90" s="5">
         <f t="shared" si="17"/>
         <v>788</v>
@@ -5627,27 +5694,27 @@
         <f t="shared" si="12"/>
         <v>289</v>
       </c>
-      <c r="F91" s="9"/>
+      <c r="F91" s="7"/>
       <c r="G91">
         <f t="shared" si="13"/>
         <v>389</v>
       </c>
-      <c r="H91" s="9"/>
+      <c r="H91" s="7"/>
       <c r="I91">
         <f t="shared" si="14"/>
         <v>489</v>
       </c>
-      <c r="J91" s="28"/>
+      <c r="J91" s="8"/>
       <c r="K91">
         <f t="shared" si="15"/>
         <v>589</v>
       </c>
-      <c r="L91" s="28"/>
+      <c r="L91" s="8"/>
       <c r="M91">
         <f t="shared" si="16"/>
         <v>689</v>
       </c>
-      <c r="N91" s="4"/>
+      <c r="N91" s="34"/>
       <c r="O91" s="5">
         <f t="shared" si="17"/>
         <v>789</v>
@@ -5678,27 +5745,27 @@
         <f t="shared" si="12"/>
         <v>290</v>
       </c>
-      <c r="F92" s="9"/>
+      <c r="F92" s="7"/>
       <c r="G92">
         <f t="shared" si="13"/>
         <v>390</v>
       </c>
-      <c r="H92" s="9"/>
+      <c r="H92" s="7"/>
       <c r="I92">
         <f t="shared" si="14"/>
         <v>490</v>
       </c>
-      <c r="J92" s="28"/>
+      <c r="J92" s="8"/>
       <c r="K92">
         <f t="shared" si="15"/>
         <v>590</v>
       </c>
-      <c r="L92" s="28"/>
+      <c r="L92" s="8"/>
       <c r="M92">
         <f t="shared" si="16"/>
         <v>690</v>
       </c>
-      <c r="N92" s="4"/>
+      <c r="N92" s="33"/>
       <c r="O92" s="5">
         <f t="shared" si="17"/>
         <v>790</v>
@@ -5718,7 +5785,7 @@
         <f t="shared" si="10"/>
         <v>91</v>
       </c>
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C93">
@@ -5729,27 +5796,27 @@
         <f t="shared" si="12"/>
         <v>291</v>
       </c>
-      <c r="F93" s="9"/>
+      <c r="F93" s="7"/>
       <c r="G93">
         <f t="shared" si="13"/>
         <v>391</v>
       </c>
-      <c r="H93" s="9"/>
+      <c r="H93" s="7"/>
       <c r="I93">
         <f t="shared" si="14"/>
         <v>491</v>
       </c>
-      <c r="J93" s="28"/>
+      <c r="J93" s="8"/>
       <c r="K93">
         <f t="shared" si="15"/>
         <v>591</v>
       </c>
-      <c r="L93" s="28"/>
-      <c r="M93">
+      <c r="L93" s="8"/>
+      <c r="M93" s="35">
         <f t="shared" si="16"/>
         <v>691</v>
       </c>
-      <c r="N93" s="4"/>
+      <c r="N93" s="32"/>
       <c r="O93" s="5">
         <f t="shared" si="17"/>
         <v>791</v>
@@ -5769,7 +5836,7 @@
         <f t="shared" si="10"/>
         <v>92</v>
       </c>
-      <c r="B94" s="13"/>
+      <c r="B94" s="9"/>
       <c r="C94">
         <f t="shared" si="11"/>
         <v>192</v>
@@ -5778,27 +5845,27 @@
         <f t="shared" si="12"/>
         <v>292</v>
       </c>
-      <c r="F94" s="9"/>
+      <c r="F94" s="7"/>
       <c r="G94">
         <f t="shared" si="13"/>
         <v>392</v>
       </c>
-      <c r="H94" s="9"/>
+      <c r="H94" s="7"/>
       <c r="I94">
         <f t="shared" si="14"/>
         <v>492</v>
       </c>
-      <c r="J94" s="28"/>
+      <c r="J94" s="8"/>
       <c r="K94">
         <f t="shared" si="15"/>
         <v>592</v>
       </c>
-      <c r="L94" s="28"/>
-      <c r="M94">
+      <c r="L94" s="8"/>
+      <c r="M94" s="35">
         <f t="shared" si="16"/>
         <v>692</v>
       </c>
-      <c r="N94" s="4"/>
+      <c r="N94" s="36"/>
       <c r="O94" s="5">
         <f t="shared" si="17"/>
         <v>792</v>
@@ -5818,7 +5885,7 @@
         <f t="shared" si="10"/>
         <v>93</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C95">
@@ -5829,27 +5896,27 @@
         <f t="shared" si="12"/>
         <v>293</v>
       </c>
-      <c r="F95" s="9"/>
+      <c r="F95" s="7"/>
       <c r="G95">
         <f t="shared" si="13"/>
         <v>393</v>
       </c>
-      <c r="H95" s="9"/>
+      <c r="H95" s="7"/>
       <c r="I95">
         <f t="shared" si="14"/>
         <v>493</v>
       </c>
-      <c r="J95" s="28"/>
+      <c r="J95" s="8"/>
       <c r="K95">
         <f t="shared" si="15"/>
         <v>593</v>
       </c>
-      <c r="L95" s="28"/>
-      <c r="M95">
+      <c r="L95" s="8"/>
+      <c r="M95" s="35">
         <f t="shared" si="16"/>
         <v>693</v>
       </c>
-      <c r="N95" s="4"/>
+      <c r="N95" s="36"/>
       <c r="O95" s="5">
         <f t="shared" si="17"/>
         <v>793</v>
@@ -5869,7 +5936,7 @@
         <f t="shared" si="10"/>
         <v>94</v>
       </c>
-      <c r="B96" s="13"/>
+      <c r="B96" s="9"/>
       <c r="C96">
         <f t="shared" si="11"/>
         <v>194</v>
@@ -5878,27 +5945,27 @@
         <f t="shared" si="12"/>
         <v>294</v>
       </c>
-      <c r="F96" s="9"/>
+      <c r="F96" s="7"/>
       <c r="G96">
         <f t="shared" si="13"/>
         <v>394</v>
       </c>
-      <c r="H96" s="9"/>
+      <c r="H96" s="7"/>
       <c r="I96">
         <f t="shared" si="14"/>
         <v>494</v>
       </c>
-      <c r="J96" s="28"/>
+      <c r="J96" s="8"/>
       <c r="K96">
         <f t="shared" si="15"/>
         <v>594</v>
       </c>
-      <c r="L96" s="28"/>
-      <c r="M96">
+      <c r="L96" s="8"/>
+      <c r="M96" s="35">
         <f t="shared" si="16"/>
         <v>694</v>
       </c>
-      <c r="N96" s="4"/>
+      <c r="N96" s="36"/>
       <c r="O96" s="5">
         <f t="shared" si="17"/>
         <v>794</v>
@@ -5929,27 +5996,27 @@
         <f t="shared" si="12"/>
         <v>295</v>
       </c>
-      <c r="F97" s="9"/>
+      <c r="F97" s="7"/>
       <c r="G97">
         <f t="shared" si="13"/>
         <v>395</v>
       </c>
-      <c r="H97" s="9"/>
+      <c r="H97" s="7"/>
       <c r="I97">
         <f t="shared" si="14"/>
         <v>495</v>
       </c>
-      <c r="J97" s="28"/>
+      <c r="J97" s="8"/>
       <c r="K97">
         <f t="shared" si="15"/>
         <v>595</v>
       </c>
-      <c r="L97" s="28"/>
-      <c r="M97">
+      <c r="L97" s="8"/>
+      <c r="M97" s="35">
         <f t="shared" si="16"/>
         <v>695</v>
       </c>
-      <c r="N97" s="4"/>
+      <c r="N97" s="36"/>
       <c r="O97" s="5">
         <f t="shared" si="17"/>
         <v>795</v>
@@ -5969,7 +6036,7 @@
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="19" t="s">
         <v>74</v>
       </c>
       <c r="C98">
@@ -5980,27 +6047,27 @@
         <f t="shared" si="12"/>
         <v>296</v>
       </c>
-      <c r="F98" s="9"/>
+      <c r="F98" s="7"/>
       <c r="G98">
         <f t="shared" si="13"/>
         <v>396</v>
       </c>
-      <c r="H98" s="9"/>
+      <c r="H98" s="7"/>
       <c r="I98">
         <f t="shared" si="14"/>
         <v>496</v>
       </c>
-      <c r="J98" s="28"/>
+      <c r="J98" s="8"/>
       <c r="K98">
         <f t="shared" si="15"/>
         <v>596</v>
       </c>
-      <c r="L98" s="28"/>
-      <c r="M98">
+      <c r="L98" s="8"/>
+      <c r="M98" s="35">
         <f t="shared" si="16"/>
         <v>696</v>
       </c>
-      <c r="N98" s="4"/>
+      <c r="N98" s="36"/>
       <c r="O98" s="5">
         <f t="shared" si="17"/>
         <v>796</v>
@@ -6020,7 +6087,7 @@
         <f t="shared" si="10"/>
         <v>97</v>
       </c>
-      <c r="B99" s="11"/>
+      <c r="B99" s="20"/>
       <c r="C99">
         <f t="shared" si="11"/>
         <v>197</v>
@@ -6029,27 +6096,27 @@
         <f t="shared" si="12"/>
         <v>297</v>
       </c>
-      <c r="F99" s="9"/>
+      <c r="F99" s="7"/>
       <c r="G99">
         <f t="shared" si="13"/>
         <v>397</v>
       </c>
-      <c r="H99" s="9"/>
+      <c r="H99" s="7"/>
       <c r="I99">
         <f t="shared" si="14"/>
         <v>497</v>
       </c>
-      <c r="J99" s="28"/>
+      <c r="J99" s="8"/>
       <c r="K99">
         <f t="shared" si="15"/>
         <v>597</v>
       </c>
-      <c r="L99" s="28"/>
-      <c r="M99">
+      <c r="L99" s="8"/>
+      <c r="M99" s="35">
         <f t="shared" si="16"/>
         <v>697</v>
       </c>
-      <c r="N99" s="4"/>
+      <c r="N99" s="36"/>
       <c r="O99" s="5">
         <f t="shared" si="17"/>
         <v>797</v>
@@ -6069,7 +6136,7 @@
         <f t="shared" si="10"/>
         <v>98</v>
       </c>
-      <c r="B100" s="11"/>
+      <c r="B100" s="20"/>
       <c r="C100">
         <f t="shared" si="11"/>
         <v>198</v>
@@ -6078,27 +6145,27 @@
         <f t="shared" si="12"/>
         <v>298</v>
       </c>
-      <c r="F100" s="9"/>
+      <c r="F100" s="7"/>
       <c r="G100">
         <f t="shared" si="13"/>
         <v>398</v>
       </c>
-      <c r="H100" s="9"/>
+      <c r="H100" s="7"/>
       <c r="I100">
         <f t="shared" si="14"/>
         <v>498</v>
       </c>
-      <c r="J100" s="28"/>
+      <c r="J100" s="8"/>
       <c r="K100">
         <f t="shared" si="15"/>
         <v>598</v>
       </c>
-      <c r="L100" s="28"/>
-      <c r="M100">
+      <c r="L100" s="8"/>
+      <c r="M100" s="35">
         <f t="shared" si="16"/>
         <v>698</v>
       </c>
-      <c r="N100" s="4"/>
+      <c r="N100" s="36"/>
       <c r="O100" s="5">
         <f t="shared" si="17"/>
         <v>798</v>
@@ -6118,7 +6185,7 @@
         <f t="shared" si="10"/>
         <v>99</v>
       </c>
-      <c r="B101" s="12"/>
+      <c r="B101" s="21"/>
       <c r="C101">
         <f t="shared" si="11"/>
         <v>199</v>
@@ -6127,27 +6194,27 @@
         <f t="shared" si="12"/>
         <v>299</v>
       </c>
-      <c r="F101" s="9"/>
+      <c r="F101" s="7"/>
       <c r="G101">
         <f t="shared" si="13"/>
         <v>399</v>
       </c>
-      <c r="H101" s="9"/>
+      <c r="H101" s="7"/>
       <c r="I101">
         <f t="shared" si="14"/>
         <v>499</v>
       </c>
-      <c r="J101" s="28"/>
+      <c r="J101" s="8"/>
       <c r="K101">
         <f t="shared" si="15"/>
         <v>599</v>
       </c>
-      <c r="L101" s="28"/>
-      <c r="M101">
+      <c r="L101" s="8"/>
+      <c r="M101" s="35">
         <f t="shared" si="16"/>
         <v>699</v>
       </c>
-      <c r="N101" s="4"/>
+      <c r="N101" s="36"/>
       <c r="O101" s="5">
         <f t="shared" si="17"/>
         <v>799</v>
@@ -6164,6 +6231,7 @@
     </row>
     <row r="102" spans="1:19">
       <c r="J102" s="4"/>
+      <c r="P102" s="4"/>
     </row>
     <row r="103" spans="1:19">
       <c r="J103" s="4"/>
@@ -6343,12 +6411,27 @@
       <c r="J161" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="J2:J26"/>
-    <mergeCell ref="J27:J51"/>
-    <mergeCell ref="J52:J101"/>
-    <mergeCell ref="L2:L51"/>
-    <mergeCell ref="L52:L101"/>
+  <mergeCells count="41">
+    <mergeCell ref="P47:P57"/>
+    <mergeCell ref="P18:P33"/>
+    <mergeCell ref="P2:P17"/>
+    <mergeCell ref="P34:P35"/>
+    <mergeCell ref="P36:P46"/>
+    <mergeCell ref="N2:N17"/>
+    <mergeCell ref="N18:N67"/>
+    <mergeCell ref="N68:N92"/>
+    <mergeCell ref="N93:N101"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B46:B84"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="D54:D57"/>
     <mergeCell ref="B93:B94"/>
     <mergeCell ref="H52:H76"/>
     <mergeCell ref="H2:H26"/>
@@ -6365,17 +6448,11 @@
     <mergeCell ref="F52:F76"/>
     <mergeCell ref="F77:F101"/>
     <mergeCell ref="B98:B101"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B46:B84"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="J2:J26"/>
+    <mergeCell ref="J27:J51"/>
+    <mergeCell ref="J52:J101"/>
+    <mergeCell ref="L2:L51"/>
+    <mergeCell ref="L52:L101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>